<commit_message>
Masterfile incl reg tables
</commit_message>
<xml_diff>
--- a/Excel/MASTER_VARIABLES_REGRESSIONS.xlsx
+++ b/Excel/MASTER_VARIABLES_REGRESSIONS.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2883" uniqueCount="600">
   <si>
     <t>Non rotated part</t>
   </si>
@@ -3005,6 +3005,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3015,6 +3018,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3028,18 +3043,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3067,9 +3070,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4935,18 +4935,18 @@
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C39" s="148" t="s">
+      <c r="C39" s="149" t="s">
         <v>494</v>
       </c>
-      <c r="D39" s="149"/>
-      <c r="E39" s="149"/>
-      <c r="F39" s="149"/>
+      <c r="D39" s="150"/>
+      <c r="E39" s="150"/>
+      <c r="F39" s="150"/>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C40" s="150"/>
-      <c r="D40" s="150"/>
-      <c r="E40" s="150"/>
-      <c r="F40" s="150"/>
+      <c r="C40" s="151"/>
+      <c r="D40" s="151"/>
+      <c r="E40" s="151"/>
+      <c r="F40" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5599,18 +5599,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="152" t="s">
         <v>444</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
-      <c r="K2" s="151"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
@@ -7372,10 +7372,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:S67"/>
+  <dimension ref="A3:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7:L40"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7416,22 +7416,22 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="152" t="s">
+      <c r="E4" s="157" t="s">
         <v>488</v>
       </c>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
-      <c r="J4" s="153"/>
-      <c r="K4" s="153"/>
-      <c r="L4" s="153"/>
-      <c r="M4" s="153"/>
-      <c r="N4" s="153"/>
-      <c r="O4" s="153"/>
-      <c r="P4" s="153"/>
-      <c r="Q4" s="153"/>
-      <c r="R4" s="153"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="158"/>
+      <c r="J4" s="158"/>
+      <c r="K4" s="158"/>
+      <c r="L4" s="158"/>
+      <c r="M4" s="158"/>
+      <c r="N4" s="158"/>
+      <c r="O4" s="158"/>
+      <c r="P4" s="158"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="158"/>
       <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -7441,34 +7441,34 @@
       <c r="D5" s="126" t="s">
         <v>382</v>
       </c>
-      <c r="E5" s="154" t="s">
+      <c r="E5" s="159" t="s">
         <v>517</v>
       </c>
-      <c r="F5" s="155"/>
-      <c r="G5" s="154" t="s">
+      <c r="F5" s="160"/>
+      <c r="G5" s="159" t="s">
         <v>518</v>
       </c>
-      <c r="H5" s="155"/>
-      <c r="I5" s="154" t="s">
+      <c r="H5" s="160"/>
+      <c r="I5" s="159" t="s">
         <v>519</v>
       </c>
-      <c r="J5" s="155"/>
-      <c r="K5" s="154" t="s">
+      <c r="J5" s="160"/>
+      <c r="K5" s="159" t="s">
         <v>520</v>
       </c>
-      <c r="L5" s="155"/>
-      <c r="M5" s="154" t="s">
+      <c r="L5" s="160"/>
+      <c r="M5" s="159" t="s">
         <v>521</v>
       </c>
-      <c r="N5" s="155"/>
-      <c r="O5" s="154" t="s">
+      <c r="N5" s="160"/>
+      <c r="O5" s="159" t="s">
         <v>522</v>
       </c>
-      <c r="P5" s="155"/>
-      <c r="Q5" s="154" t="s">
+      <c r="P5" s="160"/>
+      <c r="Q5" s="159" t="s">
         <v>523</v>
       </c>
-      <c r="R5" s="155"/>
+      <c r="R5" s="160"/>
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7499,7 +7499,7 @@
       <c r="D7" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="E7" s="169">
+      <c r="E7" s="148">
         <v>105.16</v>
       </c>
       <c r="F7" s="127">
@@ -7508,24 +7508,39 @@
       <c r="G7" s="1">
         <v>68.540000000000006</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="127">
         <v>5.22</v>
       </c>
       <c r="I7" s="1">
         <v>65.75</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="127">
         <v>5.53</v>
       </c>
       <c r="K7" s="1">
         <v>52.61</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="127">
         <v>6.08</v>
       </c>
-      <c r="N7" s="127"/>
-      <c r="P7" s="127"/>
-      <c r="R7" s="127"/>
+      <c r="M7" s="1">
+        <v>58.43</v>
+      </c>
+      <c r="N7" s="127">
+        <v>5.97</v>
+      </c>
+      <c r="O7" s="1">
+        <v>52.04</v>
+      </c>
+      <c r="P7" s="127">
+        <v>6.1</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>52.72</v>
+      </c>
+      <c r="R7" s="127">
+        <v>6.12</v>
+      </c>
       <c r="S7" s="3"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -7535,29 +7550,48 @@
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="128"/>
-      <c r="F8" s="128"/>
+      <c r="E8" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F8" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="G8" s="1">
         <v>23.53</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="127">
         <v>1.96</v>
       </c>
       <c r="I8" s="1">
         <v>23.53</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="127">
         <v>1.85</v>
       </c>
       <c r="K8" s="1">
         <v>22.88</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="127">
         <v>1.83</v>
       </c>
-      <c r="N8" s="127"/>
-      <c r="P8" s="127"/>
-      <c r="R8" s="127"/>
+      <c r="M8" s="1">
+        <v>24.38</v>
+      </c>
+      <c r="N8" s="127">
+        <v>1.94</v>
+      </c>
+      <c r="O8" s="1">
+        <v>21.33</v>
+      </c>
+      <c r="P8" s="127">
+        <v>2.04</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>21.72</v>
+      </c>
+      <c r="R8" s="127">
+        <v>1.91</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
@@ -7566,29 +7600,48 @@
       <c r="D9" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="E9" s="128"/>
-      <c r="F9" s="128"/>
+      <c r="E9" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F9" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="G9" s="1">
         <v>34.590000000000003</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="127">
         <v>4.57</v>
       </c>
       <c r="I9" s="1">
         <v>33.630000000000003</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="127">
         <v>4.5599999999999996</v>
       </c>
       <c r="K9" s="1">
         <v>25.9</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="127">
         <v>4.0199999999999996</v>
       </c>
-      <c r="N9" s="127"/>
-      <c r="P9" s="127"/>
-      <c r="R9" s="127"/>
+      <c r="M9" s="1">
+        <v>25.25</v>
+      </c>
+      <c r="N9" s="127">
+        <v>3.41</v>
+      </c>
+      <c r="O9" s="1">
+        <v>21.72</v>
+      </c>
+      <c r="P9" s="127">
+        <v>4.21</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>21.7</v>
+      </c>
+      <c r="R9" s="127">
+        <v>3.91</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
@@ -7597,29 +7650,48 @@
       <c r="D10" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E10" s="128"/>
-      <c r="F10" s="128"/>
+      <c r="E10" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F10" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="G10" s="1">
         <v>-55.5</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="127">
         <v>5.25</v>
       </c>
       <c r="I10" s="1">
         <v>-53.92</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="127">
         <v>5.52</v>
       </c>
       <c r="K10" s="1">
         <v>-45.81</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="127">
         <v>3.89</v>
       </c>
-      <c r="N10" s="127"/>
-      <c r="P10" s="127"/>
-      <c r="R10" s="127"/>
+      <c r="M10" s="1">
+        <v>-40.03</v>
+      </c>
+      <c r="N10" s="127">
+        <v>3.48</v>
+      </c>
+      <c r="O10" s="1">
+        <v>-42.04</v>
+      </c>
+      <c r="P10" s="127">
+        <v>4.75</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>-39.729999999999997</v>
+      </c>
+      <c r="R10" s="127">
+        <v>3.75</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
@@ -7628,29 +7700,48 @@
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="128"/>
-      <c r="F11" s="128"/>
+      <c r="E11" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F11" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="G11" s="1">
         <v>-9.43</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="127">
         <v>1.74</v>
       </c>
       <c r="I11" s="1">
         <v>-9.14</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="127">
         <v>1.74</v>
       </c>
       <c r="K11" s="1">
         <v>-8.57</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="127">
         <v>1.64</v>
       </c>
-      <c r="N11" s="127"/>
-      <c r="P11" s="127"/>
-      <c r="R11" s="127"/>
+      <c r="M11" s="1">
+        <v>-5.83</v>
+      </c>
+      <c r="N11" s="127">
+        <v>1.56</v>
+      </c>
+      <c r="O11" s="1">
+        <v>-6.28</v>
+      </c>
+      <c r="P11" s="127">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>-6.06</v>
+      </c>
+      <c r="R11" s="127">
+        <v>1.6</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
@@ -7659,29 +7750,48 @@
       <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="128"/>
-      <c r="F12" s="128"/>
+      <c r="E12" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F12" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="G12" s="1">
         <v>-9.06</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="127">
         <v>2.0699999999999998</v>
       </c>
       <c r="I12" s="1">
         <v>-9.35</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="127">
         <v>2.08</v>
       </c>
       <c r="K12" s="1">
         <v>-9.16</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="127">
         <v>1.92</v>
       </c>
-      <c r="N12" s="127"/>
-      <c r="P12" s="127"/>
-      <c r="R12" s="127"/>
+      <c r="M12" s="1">
+        <v>-7.69</v>
+      </c>
+      <c r="N12" s="127">
+        <v>1.87</v>
+      </c>
+      <c r="O12" s="1">
+        <v>-10.99</v>
+      </c>
+      <c r="P12" s="127">
+        <v>2.44</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>-7.11</v>
+      </c>
+      <c r="R12" s="127">
+        <v>2.09</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -7690,29 +7800,48 @@
       <c r="D13" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="E13" s="128"/>
-      <c r="F13" s="128"/>
+      <c r="E13" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F13" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="G13" s="1">
         <v>0.08</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="127">
         <v>0.01</v>
       </c>
       <c r="I13" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="127">
         <v>0.01</v>
       </c>
       <c r="K13" s="1">
         <v>0.06</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="127">
         <v>0.01</v>
       </c>
-      <c r="N13" s="127"/>
-      <c r="P13" s="127"/>
-      <c r="R13" s="127"/>
+      <c r="M13" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="N13" s="127">
+        <v>0.01</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="P13" s="127">
+        <v>0.01</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="R13" s="127">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
@@ -7721,29 +7850,48 @@
       <c r="D14" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="E14" s="128"/>
-      <c r="F14" s="128"/>
+      <c r="E14" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F14" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="G14" s="1">
         <v>8.34</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="127">
         <v>4.57</v>
       </c>
       <c r="I14" s="1">
         <v>6.32</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="127">
         <v>4.7699999999999996</v>
       </c>
       <c r="K14" s="1">
         <v>1.98</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="127">
         <v>4.54</v>
       </c>
-      <c r="N14" s="127"/>
-      <c r="P14" s="127"/>
-      <c r="R14" s="127"/>
+      <c r="M14" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="N14" s="127">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="O14" s="1">
+        <v>2.69</v>
+      </c>
+      <c r="P14" s="127">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>3.18</v>
+      </c>
+      <c r="R14" s="127">
+        <v>4.28</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
@@ -7752,29 +7900,48 @@
       <c r="D15" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="128"/>
-      <c r="F15" s="128"/>
+      <c r="E15" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F15" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="G15" s="1">
         <v>50.94</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="127">
         <v>17.61</v>
       </c>
       <c r="I15" s="1">
         <v>49.39</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="127">
         <v>18.22</v>
       </c>
       <c r="K15" s="1">
         <v>32.15</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="127">
         <v>18.440000000000001</v>
       </c>
-      <c r="N15" s="127"/>
-      <c r="P15" s="127"/>
-      <c r="R15" s="127"/>
+      <c r="M15" s="1">
+        <v>18.62</v>
+      </c>
+      <c r="N15" s="127">
+        <v>11.35</v>
+      </c>
+      <c r="O15" s="1">
+        <v>19.59</v>
+      </c>
+      <c r="P15" s="127">
+        <v>13.32</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>23.68</v>
+      </c>
+      <c r="R15" s="127">
+        <v>12.34</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
@@ -7783,29 +7950,48 @@
       <c r="D16" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="E16" s="128"/>
-      <c r="F16" s="128"/>
+      <c r="E16" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F16" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="G16" s="1">
         <v>0.04</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="127">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I16" s="1">
         <v>0.01</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="127">
         <v>0.06</v>
       </c>
       <c r="K16" s="1">
         <v>0.02</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="127">
         <v>0.06</v>
       </c>
-      <c r="N16" s="127"/>
-      <c r="P16" s="127"/>
-      <c r="R16" s="127"/>
+      <c r="M16" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="N16" s="127">
+        <v>0.06</v>
+      </c>
+      <c r="O16" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="P16" s="127">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>-0.02</v>
+      </c>
+      <c r="R16" s="127">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
@@ -7814,29 +8000,48 @@
       <c r="D17" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="E17" s="128"/>
-      <c r="F17" s="128"/>
+      <c r="E17" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F17" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="G17" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="127">
         <v>0.06</v>
       </c>
       <c r="I17" s="1">
         <v>0.15</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="127">
         <v>0.06</v>
       </c>
       <c r="K17" s="1">
         <v>0.1</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17" s="127">
         <v>0.06</v>
       </c>
-      <c r="N17" s="127"/>
-      <c r="P17" s="127"/>
-      <c r="R17" s="127"/>
+      <c r="M17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N17" s="127">
+        <v>0.06</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="P17" s="127">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="R17" s="127">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
@@ -7845,29 +8050,48 @@
       <c r="D18" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="E18" s="128"/>
-      <c r="F18" s="128"/>
+      <c r="E18" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F18" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="G18" s="1">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="127">
         <v>0.06</v>
       </c>
       <c r="I18" s="1">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="127">
         <v>0.06</v>
       </c>
       <c r="K18" s="1">
         <v>-0.2</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18" s="127">
         <v>0.06</v>
       </c>
-      <c r="N18" s="127"/>
-      <c r="P18" s="127"/>
-      <c r="R18" s="127"/>
+      <c r="M18" s="1">
+        <v>-0.12</v>
+      </c>
+      <c r="N18" s="127">
+        <v>0.06</v>
+      </c>
+      <c r="O18" s="1">
+        <v>-0.09</v>
+      </c>
+      <c r="P18" s="127">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>-0.15</v>
+      </c>
+      <c r="R18" s="127">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
@@ -7876,25 +8100,48 @@
       <c r="D19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="128"/>
-      <c r="F19" s="128"/>
-      <c r="G19" s="128"/>
-      <c r="H19" s="128"/>
+      <c r="E19" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F19" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G19" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H19" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="I19" s="1">
         <v>5.66</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="127">
         <v>6.32</v>
       </c>
       <c r="K19" s="1">
         <v>4.3499999999999996</v>
       </c>
-      <c r="L19" s="1">
+      <c r="L19" s="127">
         <v>6.28</v>
       </c>
-      <c r="N19" s="127"/>
-      <c r="P19" s="127"/>
-      <c r="R19" s="127"/>
+      <c r="M19" s="1">
+        <v>2.52</v>
+      </c>
+      <c r="N19" s="127">
+        <v>5.52</v>
+      </c>
+      <c r="O19" s="1">
+        <v>-3.75</v>
+      </c>
+      <c r="P19" s="127">
+        <v>6.76</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>5.24</v>
+      </c>
+      <c r="R19" s="127">
+        <v>5.75</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
@@ -7903,25 +8150,48 @@
       <c r="D20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="128"/>
-      <c r="F20" s="128"/>
-      <c r="G20" s="128"/>
-      <c r="H20" s="128"/>
+      <c r="E20" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F20" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G20" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H20" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="I20" s="1">
         <v>-1.92</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="127">
         <v>2.2200000000000002</v>
       </c>
       <c r="K20" s="1">
         <v>2.82</v>
       </c>
-      <c r="L20" s="1">
+      <c r="L20" s="127">
         <v>2.2400000000000002</v>
       </c>
-      <c r="N20" s="127"/>
-      <c r="P20" s="127"/>
-      <c r="R20" s="127"/>
+      <c r="M20" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="N20" s="127">
+        <v>1.87</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="P20" s="127">
+        <v>2.02</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="R20" s="127">
+        <v>1.76</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="130"/>
@@ -7930,25 +8200,48 @@
       <c r="D21" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="E21" s="128"/>
-      <c r="F21" s="128"/>
-      <c r="G21" s="128"/>
-      <c r="H21" s="128"/>
+      <c r="E21" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F21" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G21" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H21" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="I21" s="1">
         <v>10.58</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="127">
         <v>8.5500000000000007</v>
       </c>
       <c r="K21" s="1">
         <v>3.95</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L21" s="127">
         <v>8.6300000000000008</v>
       </c>
-      <c r="N21" s="127"/>
-      <c r="P21" s="127"/>
-      <c r="R21" s="127"/>
+      <c r="M21" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="N21" s="127">
+        <v>9.11</v>
+      </c>
+      <c r="O21" s="1">
+        <v>7.33</v>
+      </c>
+      <c r="P21" s="127">
+        <v>10.6</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="R21" s="127">
+        <v>8.73</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="130"/>
@@ -7957,25 +8250,48 @@
       <c r="D22" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="E22" s="128"/>
-      <c r="F22" s="128"/>
-      <c r="G22" s="128"/>
-      <c r="H22" s="128"/>
+      <c r="E22" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F22" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G22" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H22" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="I22" s="1">
         <v>-14.89</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="127">
         <v>10.8</v>
       </c>
       <c r="K22" s="1">
         <v>-33.18</v>
       </c>
-      <c r="L22" s="1">
+      <c r="L22" s="127">
         <v>12.25</v>
       </c>
-      <c r="N22" s="127"/>
-      <c r="P22" s="127"/>
-      <c r="R22" s="127"/>
+      <c r="M22" s="1">
+        <v>-9.31</v>
+      </c>
+      <c r="N22" s="127">
+        <v>13.19</v>
+      </c>
+      <c r="O22" s="1">
+        <v>-26.84</v>
+      </c>
+      <c r="P22" s="127">
+        <v>11.87</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>-8.41</v>
+      </c>
+      <c r="R22" s="127">
+        <v>11.76</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
@@ -7984,25 +8300,48 @@
       <c r="D23" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="E23" s="128"/>
-      <c r="F23" s="128"/>
-      <c r="G23" s="128"/>
-      <c r="H23" s="128"/>
+      <c r="E23" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F23" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G23" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H23" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="I23" s="1">
         <v>12.81</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="127">
         <v>5.79</v>
       </c>
       <c r="K23" s="1">
         <v>11.05</v>
       </c>
-      <c r="L23" s="1">
+      <c r="L23" s="127">
         <v>6.17</v>
       </c>
-      <c r="N23" s="127"/>
-      <c r="P23" s="127"/>
-      <c r="R23" s="127"/>
+      <c r="M23" s="1">
+        <v>13</v>
+      </c>
+      <c r="N23" s="127">
+        <v>5.79</v>
+      </c>
+      <c r="O23" s="1">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="P23" s="127">
+        <v>5.98</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>10.31</v>
+      </c>
+      <c r="R23" s="127">
+        <v>5.72</v>
+      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
@@ -8011,25 +8350,48 @@
       <c r="D24" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="E24" s="128"/>
-      <c r="F24" s="128"/>
-      <c r="G24" s="128"/>
-      <c r="H24" s="128"/>
+      <c r="E24" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F24" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G24" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H24" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="I24" s="1">
         <v>4.43</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="127">
         <v>7.52</v>
       </c>
       <c r="K24" s="1">
         <v>-0.52</v>
       </c>
-      <c r="L24" s="1">
+      <c r="L24" s="127">
         <v>7.2</v>
       </c>
-      <c r="N24" s="127"/>
-      <c r="P24" s="127"/>
-      <c r="R24" s="127"/>
+      <c r="M24" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="N24" s="127">
+        <v>5.78</v>
+      </c>
+      <c r="O24" s="1">
+        <v>-1.36</v>
+      </c>
+      <c r="P24" s="127">
+        <v>7.16</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="R24" s="127">
+        <v>6.22</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
@@ -8038,25 +8400,48 @@
       <c r="D25" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="E25" s="128"/>
-      <c r="F25" s="128"/>
-      <c r="G25" s="128"/>
-      <c r="H25" s="128"/>
+      <c r="E25" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F25" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G25" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H25" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="I25" s="1">
         <v>-3.26</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="127">
         <v>9.9499999999999993</v>
       </c>
       <c r="K25" s="1">
         <v>-7.5</v>
       </c>
-      <c r="L25" s="1">
+      <c r="L25" s="127">
         <v>10.48</v>
       </c>
-      <c r="N25" s="127"/>
-      <c r="P25" s="127"/>
-      <c r="R25" s="127"/>
+      <c r="M25" s="1">
+        <v>-4.5599999999999996</v>
+      </c>
+      <c r="N25" s="127">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="O25" s="1">
+        <v>-2.52</v>
+      </c>
+      <c r="P25" s="127">
+        <v>8.76</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>-2.16</v>
+      </c>
+      <c r="R25" s="127">
+        <v>8.7899999999999991</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
@@ -8065,25 +8450,48 @@
       <c r="D26" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="E26" s="128"/>
-      <c r="F26" s="128"/>
-      <c r="G26" s="128"/>
-      <c r="H26" s="128"/>
+      <c r="E26" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F26" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G26" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H26" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="I26" s="1">
         <v>6.35</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26" s="127">
         <v>5.28</v>
       </c>
       <c r="K26" s="1">
         <v>3.09</v>
       </c>
-      <c r="L26" s="1">
+      <c r="L26" s="127">
         <v>5.2</v>
       </c>
-      <c r="N26" s="127"/>
-      <c r="P26" s="127"/>
-      <c r="R26" s="127"/>
+      <c r="M26" s="1">
+        <v>7.22</v>
+      </c>
+      <c r="N26" s="127">
+        <v>4.24</v>
+      </c>
+      <c r="O26" s="1">
+        <v>6.08</v>
+      </c>
+      <c r="P26" s="127">
+        <v>4.82</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="R26" s="127">
+        <v>4.29</v>
+      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
@@ -8092,20 +8500,48 @@
       <c r="D27" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="E27" s="128"/>
-      <c r="F27" s="128"/>
-      <c r="G27" s="128"/>
-      <c r="H27" s="128"/>
-      <c r="J27" s="127"/>
+      <c r="E27" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F27" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G27" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H27" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I27" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J27" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K27" s="1">
         <v>-6.31</v>
       </c>
-      <c r="L27" s="1">
+      <c r="L27" s="127">
         <v>4.21</v>
       </c>
-      <c r="N27" s="127"/>
-      <c r="P27" s="127"/>
-      <c r="R27" s="127"/>
+      <c r="M27" s="1">
+        <v>-5.47</v>
+      </c>
+      <c r="N27" s="127">
+        <v>3.61</v>
+      </c>
+      <c r="O27" s="1">
+        <v>-7.44</v>
+      </c>
+      <c r="P27" s="127">
+        <v>4.04</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>-5.75</v>
+      </c>
+      <c r="R27" s="127">
+        <v>3.81</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
@@ -8114,20 +8550,48 @@
       <c r="D28" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E28" s="128"/>
-      <c r="F28" s="128"/>
-      <c r="G28" s="128"/>
-      <c r="H28" s="128"/>
-      <c r="J28" s="127"/>
+      <c r="E28" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F28" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G28" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H28" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I28" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J28" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K28" s="1">
         <v>0.86</v>
       </c>
-      <c r="L28" s="1">
+      <c r="L28" s="127">
         <v>0.24</v>
       </c>
-      <c r="N28" s="127"/>
-      <c r="P28" s="127"/>
-      <c r="R28" s="127"/>
+      <c r="M28" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="N28" s="127">
+        <v>0.24</v>
+      </c>
+      <c r="O28" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="P28" s="127">
+        <v>0.3</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="R28" s="127">
+        <v>0.23</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
@@ -8136,20 +8600,48 @@
       <c r="D29" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E29" s="128"/>
-      <c r="F29" s="128"/>
-      <c r="G29" s="128"/>
-      <c r="H29" s="128"/>
-      <c r="J29" s="127"/>
+      <c r="E29" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F29" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G29" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H29" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I29" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J29" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K29" s="1">
         <v>12.94</v>
       </c>
-      <c r="L29" s="1">
+      <c r="L29" s="127">
         <v>6.52</v>
       </c>
-      <c r="N29" s="127"/>
-      <c r="P29" s="127"/>
-      <c r="R29" s="127"/>
+      <c r="M29" s="1">
+        <v>14.49</v>
+      </c>
+      <c r="N29" s="127">
+        <v>5.51</v>
+      </c>
+      <c r="O29" s="1">
+        <v>18.02</v>
+      </c>
+      <c r="P29" s="127">
+        <v>6.16</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>15.38</v>
+      </c>
+      <c r="R29" s="127">
+        <v>5.95</v>
+      </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
@@ -8158,21 +8650,48 @@
       <c r="D30" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E30" s="128"/>
-      <c r="F30" s="128"/>
-      <c r="G30" s="128"/>
-      <c r="H30" s="128"/>
-      <c r="I30" s="128"/>
-      <c r="J30" s="128"/>
+      <c r="E30" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F30" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G30" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H30" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I30" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J30" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K30" s="1">
         <v>6.18</v>
       </c>
-      <c r="L30" s="1">
+      <c r="L30" s="127">
         <v>3.24</v>
       </c>
-      <c r="N30" s="127"/>
-      <c r="P30" s="127"/>
-      <c r="R30" s="127"/>
+      <c r="M30" s="1">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="N30" s="127">
+        <v>2.68</v>
+      </c>
+      <c r="O30" s="1">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="P30" s="127">
+        <v>2.85</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="R30" s="127">
+        <v>2.62</v>
+      </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
@@ -8181,21 +8700,48 @@
       <c r="D31" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E31" s="128"/>
-      <c r="F31" s="128"/>
-      <c r="G31" s="128"/>
-      <c r="H31" s="128"/>
-      <c r="I31" s="128"/>
-      <c r="J31" s="128"/>
+      <c r="E31" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F31" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G31" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H31" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I31" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J31" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K31" s="1">
         <v>1.21</v>
       </c>
-      <c r="L31" s="1">
+      <c r="L31" s="127">
         <v>2.61</v>
       </c>
-      <c r="N31" s="127"/>
-      <c r="P31" s="127"/>
-      <c r="R31" s="127"/>
+      <c r="M31" s="1">
+        <v>1.44</v>
+      </c>
+      <c r="N31" s="127">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="O31" s="1">
+        <v>1.92</v>
+      </c>
+      <c r="P31" s="127">
+        <v>2.65</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="R31" s="127">
+        <v>2.37</v>
+      </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
@@ -8204,21 +8750,48 @@
       <c r="D32" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E32" s="128"/>
-      <c r="F32" s="128"/>
-      <c r="G32" s="128"/>
-      <c r="H32" s="128"/>
-      <c r="I32" s="128"/>
-      <c r="J32" s="128"/>
+      <c r="E32" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F32" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G32" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H32" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I32" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J32" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K32" s="1">
         <v>13.37</v>
       </c>
-      <c r="L32" s="1">
+      <c r="L32" s="127">
         <v>5</v>
       </c>
-      <c r="N32" s="127"/>
-      <c r="P32" s="127"/>
-      <c r="R32" s="127"/>
+      <c r="M32" s="1">
+        <v>12.72</v>
+      </c>
+      <c r="N32" s="127">
+        <v>4</v>
+      </c>
+      <c r="O32" s="1">
+        <v>10.41</v>
+      </c>
+      <c r="P32" s="127">
+        <v>4.43</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>12.82</v>
+      </c>
+      <c r="R32" s="127">
+        <v>3.93</v>
+      </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
@@ -8227,21 +8800,48 @@
       <c r="D33" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E33" s="128"/>
-      <c r="F33" s="128"/>
-      <c r="G33" s="128"/>
-      <c r="H33" s="128"/>
-      <c r="I33" s="128"/>
-      <c r="J33" s="128"/>
+      <c r="E33" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F33" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G33" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H33" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I33" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J33" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K33" s="1">
         <v>11.57</v>
       </c>
-      <c r="L33" s="1">
+      <c r="L33" s="127">
         <v>5.28</v>
       </c>
-      <c r="N33" s="127"/>
-      <c r="P33" s="127"/>
-      <c r="R33" s="127"/>
+      <c r="M33" s="1">
+        <v>8.48</v>
+      </c>
+      <c r="N33" s="127">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="O33" s="1">
+        <v>11.32</v>
+      </c>
+      <c r="P33" s="127">
+        <v>5.37</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>6.71</v>
+      </c>
+      <c r="R33" s="127">
+        <v>5.05</v>
+      </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
@@ -8250,21 +8850,48 @@
       <c r="D34" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E34" s="128"/>
-      <c r="F34" s="128"/>
-      <c r="G34" s="128"/>
-      <c r="H34" s="128"/>
-      <c r="I34" s="128"/>
-      <c r="J34" s="128"/>
+      <c r="E34" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F34" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G34" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H34" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I34" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J34" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K34" s="1">
         <v>1.81</v>
       </c>
-      <c r="L34" s="1">
+      <c r="L34" s="127">
         <v>15.17</v>
       </c>
-      <c r="N34" s="127"/>
-      <c r="P34" s="127"/>
-      <c r="R34" s="127"/>
+      <c r="M34" s="1">
+        <v>-3.33</v>
+      </c>
+      <c r="N34" s="127">
+        <v>11.81</v>
+      </c>
+      <c r="O34" s="1">
+        <v>-8.39</v>
+      </c>
+      <c r="P34" s="127">
+        <v>11.23</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>-8.98</v>
+      </c>
+      <c r="R34" s="127">
+        <v>11.41</v>
+      </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
@@ -8273,21 +8900,48 @@
       <c r="D35" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="E35" s="128"/>
-      <c r="F35" s="128"/>
-      <c r="G35" s="128"/>
-      <c r="H35" s="128"/>
-      <c r="I35" s="128"/>
-      <c r="J35" s="128"/>
+      <c r="E35" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F35" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G35" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H35" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I35" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J35" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K35" s="1">
         <v>9.3699999999999992</v>
       </c>
-      <c r="L35" s="1">
+      <c r="L35" s="127">
         <v>6.2</v>
       </c>
-      <c r="N35" s="127"/>
-      <c r="P35" s="127"/>
-      <c r="R35" s="127"/>
+      <c r="M35" s="1">
+        <v>11.66</v>
+      </c>
+      <c r="N35" s="127">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="O35" s="1">
+        <v>13.58</v>
+      </c>
+      <c r="P35" s="127">
+        <v>5.91</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>10.15</v>
+      </c>
+      <c r="R35" s="127">
+        <v>5.61</v>
+      </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
@@ -8296,21 +8950,48 @@
       <c r="D36" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="E36" s="128"/>
-      <c r="F36" s="128"/>
-      <c r="G36" s="128"/>
-      <c r="H36" s="128"/>
-      <c r="I36" s="128"/>
-      <c r="J36" s="128"/>
+      <c r="E36" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F36" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G36" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H36" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I36" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J36" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K36" s="1">
         <v>4.93</v>
       </c>
-      <c r="L36" s="1">
+      <c r="L36" s="127">
         <v>5.65</v>
       </c>
-      <c r="N36" s="127"/>
-      <c r="P36" s="127"/>
-      <c r="R36" s="127"/>
+      <c r="M36" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N36" s="127">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="O36" s="1">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="P36" s="127">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>4.93</v>
+      </c>
+      <c r="R36" s="127">
+        <v>4.34</v>
+      </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
@@ -8319,21 +9000,48 @@
       <c r="D37" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E37" s="128"/>
-      <c r="F37" s="128"/>
-      <c r="G37" s="128"/>
-      <c r="H37" s="128"/>
-      <c r="I37" s="128"/>
-      <c r="J37" s="128"/>
+      <c r="E37" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F37" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G37" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H37" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I37" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J37" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K37" s="1">
         <v>1.62</v>
       </c>
-      <c r="L37" s="1">
+      <c r="L37" s="127">
         <v>2.57</v>
       </c>
-      <c r="N37" s="127"/>
-      <c r="P37" s="127"/>
-      <c r="R37" s="127"/>
+      <c r="M37" s="1">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="N37" s="127">
+        <v>2</v>
+      </c>
+      <c r="O37" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="P37" s="127">
+        <v>2.11</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="R37" s="127">
+        <v>2.0699999999999998</v>
+      </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
@@ -8342,21 +9050,48 @@
       <c r="D38" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="E38" s="128"/>
-      <c r="F38" s="128"/>
-      <c r="G38" s="128"/>
-      <c r="H38" s="128"/>
-      <c r="I38" s="128"/>
-      <c r="J38" s="128"/>
+      <c r="E38" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F38" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G38" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H38" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I38" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J38" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K38" s="1">
         <v>3.25</v>
       </c>
-      <c r="L38" s="1">
+      <c r="L38" s="127">
         <v>8.56</v>
       </c>
-      <c r="N38" s="127"/>
-      <c r="P38" s="127"/>
-      <c r="R38" s="127"/>
+      <c r="M38" s="1">
+        <v>-7.26</v>
+      </c>
+      <c r="N38" s="127">
+        <v>6.9</v>
+      </c>
+      <c r="O38" s="1">
+        <v>-10.28</v>
+      </c>
+      <c r="P38" s="127">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>-6.29</v>
+      </c>
+      <c r="R38" s="127">
+        <v>6.97</v>
+      </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
@@ -8365,21 +9100,48 @@
       <c r="D39" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E39" s="128"/>
-      <c r="F39" s="128"/>
-      <c r="G39" s="128"/>
-      <c r="H39" s="128"/>
-      <c r="I39" s="128"/>
-      <c r="J39" s="128"/>
+      <c r="E39" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F39" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G39" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H39" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I39" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J39" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K39" s="1">
         <v>2.08</v>
       </c>
-      <c r="L39" s="1">
+      <c r="L39" s="127">
         <v>3.31</v>
       </c>
-      <c r="N39" s="127"/>
-      <c r="P39" s="127"/>
-      <c r="R39" s="127"/>
+      <c r="M39" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="N39" s="127">
+        <v>2.87</v>
+      </c>
+      <c r="O39" s="1">
+        <v>-0.37</v>
+      </c>
+      <c r="P39" s="127">
+        <v>3.21</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="R39" s="127">
+        <v>3.19</v>
+      </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
@@ -8388,826 +9150,567 @@
       <c r="D40" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E40" s="128"/>
-      <c r="F40" s="128"/>
-      <c r="G40" s="128"/>
-      <c r="H40" s="128"/>
-      <c r="I40" s="128"/>
-      <c r="J40" s="128"/>
+      <c r="E40" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F40" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G40" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H40" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I40" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J40" s="128" t="s">
+        <v>526</v>
+      </c>
       <c r="K40" s="1">
         <v>-1.97</v>
       </c>
-      <c r="L40" s="1">
+      <c r="L40" s="127">
         <v>2.92</v>
       </c>
-      <c r="N40" s="127"/>
-      <c r="P40" s="127"/>
-      <c r="R40" s="127"/>
+      <c r="M40" s="1">
+        <v>-1.94</v>
+      </c>
+      <c r="N40" s="127">
+        <v>2.71</v>
+      </c>
+      <c r="O40" s="1">
+        <v>-1.28</v>
+      </c>
+      <c r="P40" s="127">
+        <v>2.84</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>-1.68</v>
+      </c>
+      <c r="R40" s="127">
+        <v>2.71</v>
+      </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="E41" s="128"/>
-      <c r="F41" s="128"/>
-      <c r="G41" s="128"/>
-      <c r="H41" s="128"/>
-      <c r="I41" s="128"/>
-      <c r="J41" s="128"/>
-      <c r="L41" s="127"/>
-      <c r="N41" s="127"/>
-      <c r="P41" s="127"/>
-      <c r="R41" s="127"/>
+      <c r="D41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F41" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G41" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H41" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I41" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J41" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="K41" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="L41" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="M41" s="1">
+        <v>7.84</v>
+      </c>
+      <c r="N41" s="127">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="O41" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="P41" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q41" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="R41" s="128" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
-      <c r="E42" s="128"/>
-      <c r="F42" s="128"/>
-      <c r="G42" s="128"/>
-      <c r="H42" s="128"/>
-      <c r="I42" s="128"/>
-      <c r="J42" s="128"/>
-      <c r="L42" s="127"/>
-      <c r="N42" s="127"/>
-      <c r="P42" s="127"/>
-      <c r="R42" s="127"/>
+      <c r="D42" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="E42" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F42" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G42" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H42" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I42" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J42" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="K42" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="L42" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="M42" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="N42" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="O42" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="P42" s="127">
+        <v>0.71</v>
+      </c>
+      <c r="Q42" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="R42" s="128" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="E43" s="128"/>
-      <c r="F43" s="128"/>
-      <c r="G43" s="128"/>
-      <c r="H43" s="128"/>
-      <c r="I43" s="128"/>
-      <c r="J43" s="128"/>
-      <c r="K43" s="128"/>
-      <c r="L43" s="128"/>
-      <c r="N43" s="127"/>
-      <c r="O43" s="128"/>
-      <c r="P43" s="128"/>
-      <c r="Q43" s="128"/>
-      <c r="R43" s="128"/>
+      <c r="D43" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E43" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F43" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G43" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H43" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I43" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J43" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="K43" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="L43" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="M43" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="N43" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="O43" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="P43" s="127">
+        <v>0.22</v>
+      </c>
+      <c r="Q43" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="R43" s="128" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="E44" s="128"/>
-      <c r="F44" s="128"/>
-      <c r="G44" s="128"/>
-      <c r="H44" s="128"/>
-      <c r="I44" s="128"/>
-      <c r="J44" s="128"/>
-      <c r="K44" s="128"/>
-      <c r="L44" s="128"/>
-      <c r="N44" s="127"/>
-      <c r="O44" s="128"/>
-      <c r="P44" s="128"/>
-      <c r="Q44" s="128"/>
-      <c r="R44" s="128"/>
+      <c r="D44" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="K44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="L44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="M44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="N44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="O44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="P44" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>-6.96</v>
+      </c>
+      <c r="R44" s="127">
+        <v>1.89</v>
+      </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
-      <c r="E45" s="128"/>
-      <c r="F45" s="128"/>
-      <c r="G45" s="128"/>
-      <c r="H45" s="128"/>
-      <c r="I45" s="128"/>
-      <c r="J45" s="128"/>
-      <c r="K45" s="128"/>
-      <c r="L45" s="128"/>
-      <c r="N45" s="127"/>
-      <c r="O45" s="128"/>
-      <c r="P45" s="128"/>
-      <c r="Q45" s="128"/>
-      <c r="R45" s="128"/>
+      <c r="D45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="K45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="L45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="M45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="N45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="O45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="P45" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>10.17</v>
+      </c>
+      <c r="R45" s="127">
+        <v>1.1100000000000001</v>
+      </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
-      <c r="E46" s="128"/>
-      <c r="F46" s="128"/>
-      <c r="G46" s="128"/>
-      <c r="H46" s="128"/>
-      <c r="I46" s="128"/>
-      <c r="J46" s="128"/>
-      <c r="K46" s="128"/>
-      <c r="L46" s="128"/>
-      <c r="N46" s="127"/>
-      <c r="O46" s="128"/>
-      <c r="P46" s="128"/>
-      <c r="Q46" s="128"/>
-      <c r="R46" s="128" t="s">
-        <v>526</v>
+      <c r="D46" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="K46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="L46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="M46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="N46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="O46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="P46" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>-0.46</v>
+      </c>
+      <c r="R46" s="127">
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="E47" s="128"/>
-      <c r="F47" s="128"/>
-      <c r="G47" s="128"/>
-      <c r="H47" s="128"/>
-      <c r="I47" s="128"/>
-      <c r="J47" s="128"/>
-      <c r="K47" s="128"/>
-      <c r="L47" s="128"/>
-      <c r="N47" s="127"/>
-      <c r="O47" s="128"/>
-      <c r="P47" s="128"/>
-      <c r="Q47" s="128"/>
-      <c r="R47" s="128" t="s">
-        <v>526</v>
+      <c r="D47" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="K47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="L47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="M47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="N47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="O47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="P47" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>-6.75</v>
+      </c>
+      <c r="R47" s="127">
+        <v>1.07</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
-      <c r="E48" s="128"/>
-      <c r="F48" s="128"/>
-      <c r="G48" s="128"/>
-      <c r="H48" s="128"/>
-      <c r="I48" s="128"/>
-      <c r="J48" s="128"/>
-      <c r="K48" s="128"/>
-      <c r="L48" s="128"/>
-      <c r="N48" s="127"/>
-      <c r="O48" s="128"/>
-      <c r="P48" s="128"/>
-      <c r="Q48" s="128"/>
-      <c r="R48" s="128" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D48" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="F48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="G48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="H48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="I48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="J48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="K48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="L48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="M48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="N48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="O48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="P48" s="128" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>-13.31</v>
+      </c>
+      <c r="R48" s="127">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
-      <c r="E49" s="128"/>
-      <c r="F49" s="128"/>
-      <c r="G49" s="128"/>
-      <c r="H49" s="128"/>
-      <c r="I49" s="128"/>
-      <c r="J49" s="128"/>
-      <c r="K49" s="128"/>
-      <c r="L49" s="128"/>
-      <c r="N49" s="127"/>
-      <c r="O49" s="128"/>
-      <c r="P49" s="128"/>
-      <c r="Q49" s="128"/>
-      <c r="R49" s="128" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D49" s="131" t="s">
+        <v>545</v>
+      </c>
+      <c r="E49" s="155">
+        <v>19.61</v>
+      </c>
+      <c r="F49" s="153"/>
+      <c r="G49" s="156">
+        <v>38.72</v>
+      </c>
+      <c r="H49" s="153"/>
+      <c r="I49" s="153">
+        <v>39.26</v>
+      </c>
+      <c r="J49" s="153"/>
+      <c r="K49" s="153">
+        <v>43.09</v>
+      </c>
+      <c r="L49" s="153"/>
+      <c r="M49" s="153">
+        <v>42.69</v>
+      </c>
+      <c r="N49" s="153"/>
+      <c r="O49" s="153">
+        <v>39.82</v>
+      </c>
+      <c r="P49" s="153"/>
+      <c r="Q49" s="153">
+        <v>43.62</v>
+      </c>
+      <c r="R49" s="153"/>
+    </row>
+    <row r="50" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
-      <c r="E50" s="128"/>
-      <c r="F50" s="128"/>
-      <c r="G50" s="128"/>
-      <c r="H50" s="128"/>
-      <c r="I50" s="128"/>
-      <c r="J50" s="128"/>
-      <c r="K50" s="128"/>
-      <c r="L50" s="128"/>
-      <c r="M50" s="128"/>
-      <c r="N50" s="128"/>
-      <c r="P50" s="127"/>
-      <c r="Q50" s="128"/>
-      <c r="R50" s="128" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D50" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="E50" s="155">
+        <v>48483</v>
+      </c>
+      <c r="F50" s="153"/>
+      <c r="G50" s="155">
+        <v>18474</v>
+      </c>
+      <c r="H50" s="153"/>
+      <c r="I50" s="155">
+        <v>18474</v>
+      </c>
+      <c r="J50" s="153"/>
+      <c r="K50" s="155">
+        <v>18474</v>
+      </c>
+      <c r="L50" s="153"/>
+      <c r="M50" s="153">
+        <v>17506</v>
+      </c>
+      <c r="N50" s="153"/>
+      <c r="O50" s="153">
+        <v>11843</v>
+      </c>
+      <c r="P50" s="153"/>
+      <c r="Q50" s="153">
+        <v>16829</v>
+      </c>
+      <c r="R50" s="153"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
-      <c r="E51" s="128"/>
-      <c r="F51" s="128"/>
-      <c r="G51" s="128"/>
-      <c r="H51" s="128"/>
-      <c r="I51" s="128"/>
-      <c r="J51" s="128"/>
-      <c r="K51" s="128"/>
-      <c r="L51" s="128"/>
-      <c r="M51" s="128"/>
-      <c r="N51" s="128"/>
-      <c r="P51" s="127"/>
-      <c r="Q51" s="128"/>
-      <c r="R51" s="128" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="E52" s="128"/>
-      <c r="F52" s="128"/>
-      <c r="G52" s="128"/>
-      <c r="H52" s="128"/>
-      <c r="I52" s="128"/>
-      <c r="J52" s="128"/>
-      <c r="K52" s="128"/>
-      <c r="L52" s="128"/>
-      <c r="M52" s="128"/>
-      <c r="N52" s="128"/>
-      <c r="P52" s="127"/>
-      <c r="Q52" s="128"/>
-      <c r="R52" s="128" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="E53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="F53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="G53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="H53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="I53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="J53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="K53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="L53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="M53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="N53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="O53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="P53" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="R53" s="127"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="E54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="F54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="G54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="H54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="I54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="J54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="K54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="L54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="M54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="N54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="O54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="P54" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="R54" s="127"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="E55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="F55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="G55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="H55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="I55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="J55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="K55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="L55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="M55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="N55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="O55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="P55" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="R55" s="127"/>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="E56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="F56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="G56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="H56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="I56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="J56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="K56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="L56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="M56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="N56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="O56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="P56" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="R56" s="127"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="E57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="F57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="G57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="H57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="I57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="J57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="K57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="L57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="M57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="N57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="O57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="P57" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="R57" s="127"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="E58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="F58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="G58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="H58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="I58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="J58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="K58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="L58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="M58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="N58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="O58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="P58" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="R58" s="127"/>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="E59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="F59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="G59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="H59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="I59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="J59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="K59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="L59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="M59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="N59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="O59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="P59" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="R59" s="127"/>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="E60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="F60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="G60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="H60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="I60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="J60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="K60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="L60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="M60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="N60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="O60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="P60" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="R60" s="127"/>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="E61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="F61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="G61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="H61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="I61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="J61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="K61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="L61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="M61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="N61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="O61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="P61" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="R61" s="127"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="E62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="F62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="G62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="H62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="I62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="J62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="K62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="L62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="M62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="N62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="O62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="P62" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="R62" s="127"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="E63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="F63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="G63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="H63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="I63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="J63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="K63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="L63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="M63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="N63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="O63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="P63" s="128" t="s">
-        <v>526</v>
-      </c>
-      <c r="R63" s="127"/>
-    </row>
-    <row r="64" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="131" t="s">
-        <v>545</v>
-      </c>
-      <c r="E64" s="158">
-        <v>19.61</v>
-      </c>
-      <c r="F64" s="157"/>
-      <c r="G64" s="159">
-        <v>38.72</v>
-      </c>
-      <c r="H64" s="157"/>
-      <c r="I64" s="156">
-        <v>39.26</v>
-      </c>
-      <c r="J64" s="157"/>
-      <c r="K64" s="156"/>
-      <c r="L64" s="157"/>
-      <c r="M64" s="156"/>
-      <c r="N64" s="157"/>
-      <c r="O64" s="156"/>
-      <c r="P64" s="157"/>
-      <c r="Q64" s="156"/>
-      <c r="R64" s="157"/>
-    </row>
-    <row r="65" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="E65" s="158">
-        <v>48483</v>
-      </c>
-      <c r="F65" s="157"/>
-      <c r="G65" s="158">
-        <v>18474</v>
-      </c>
-      <c r="H65" s="157"/>
-      <c r="I65" s="158">
-        <v>18474</v>
-      </c>
-      <c r="J65" s="157"/>
-      <c r="K65" s="158">
-        <v>18474</v>
-      </c>
-      <c r="L65" s="157"/>
-      <c r="M65" s="156"/>
-      <c r="N65" s="157"/>
-      <c r="O65" s="156"/>
-      <c r="P65" s="157"/>
-      <c r="Q65" s="156"/>
-      <c r="R65" s="157"/>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="3"/>
-      <c r="K66" s="3"/>
-      <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
-      <c r="N66" s="3"/>
-      <c r="O66" s="3"/>
-      <c r="P66" s="3"/>
-      <c r="Q66" s="3"/>
-      <c r="R66" s="3"/>
-      <c r="S66" s="3"/>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
-      <c r="M67" s="3"/>
-      <c r="N67" s="3"/>
-      <c r="O67" s="3"/>
-      <c r="P67" s="3"/>
-      <c r="Q67" s="3"/>
-      <c r="R67" s="3"/>
-      <c r="S67" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="Q64:R64"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="M65:N65"/>
-    <mergeCell ref="O65:P65"/>
-    <mergeCell ref="Q65:R65"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="O64:P64"/>
     <mergeCell ref="E4:R4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
@@ -9216,6 +9719,20 @@
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="O50:P50"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="O49:P49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9241,17 +9758,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="152" t="s">
         <v>455</v>
       </c>
-      <c r="C4" s="151"/>
-      <c r="D4" s="151"/>
-      <c r="E4" s="151"/>
-      <c r="F4" s="151"/>
-      <c r="G4" s="151"/>
-      <c r="H4" s="151"/>
-      <c r="I4" s="151"/>
-      <c r="J4" s="151"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
@@ -10032,7 +10549,7 @@
       <c r="B15" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="C15" s="160" t="s">
+      <c r="C15" s="161" t="s">
         <v>173</v>
       </c>
     </row>
@@ -10040,43 +10557,43 @@
       <c r="B16" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="C16" s="161"/>
+      <c r="C16" s="162"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="161"/>
+      <c r="C17" s="162"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C18" s="161"/>
+      <c r="C18" s="162"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="C19" s="161"/>
+      <c r="C19" s="162"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="C20" s="161"/>
+      <c r="C20" s="162"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C21" s="161"/>
+      <c r="C21" s="162"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C22" s="162"/>
+      <c r="C22" s="163"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="12" t="s">
@@ -10675,32 +11192,32 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="164" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="164"/>
-      <c r="D4" s="163" t="s">
+      <c r="C4" s="165"/>
+      <c r="D4" s="164" t="s">
         <v>277</v>
       </c>
-      <c r="E4" s="164"/>
-      <c r="F4" s="165" t="s">
+      <c r="E4" s="165"/>
+      <c r="F4" s="166" t="s">
         <v>278</v>
       </c>
-      <c r="G4" s="164"/>
+      <c r="G4" s="165"/>
     </row>
     <row r="5" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="166" t="s">
+      <c r="B5" s="167" t="s">
         <v>279</v>
       </c>
-      <c r="C5" s="164"/>
-      <c r="D5" s="166" t="s">
+      <c r="C5" s="165"/>
+      <c r="D5" s="167" t="s">
         <v>280</v>
       </c>
-      <c r="E5" s="164"/>
-      <c r="F5" s="167" t="s">
+      <c r="E5" s="165"/>
+      <c r="F5" s="168" t="s">
         <v>281</v>
       </c>
-      <c r="G5" s="164"/>
+      <c r="G5" s="165"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
@@ -11939,18 +12456,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="152" t="s">
         <v>474</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
-      <c r="K2" s="151"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="102" t="s">
@@ -13773,17 +14290,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B3" s="168" t="s">
+      <c r="B3" s="169" t="s">
         <v>479</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="168"/>
-      <c r="J3" s="168"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
@@ -18793,7 +19310,7 @@
       <c r="B15" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="C15" s="160" t="s">
+      <c r="C15" s="161" t="s">
         <v>173</v>
       </c>
     </row>
@@ -18801,43 +19318,43 @@
       <c r="B16" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="C16" s="161"/>
+      <c r="C16" s="162"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="161"/>
+      <c r="C17" s="162"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C18" s="161"/>
+      <c r="C18" s="162"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="C19" s="161"/>
+      <c r="C19" s="162"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="C20" s="161"/>
+      <c r="C20" s="162"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C21" s="161"/>
+      <c r="C21" s="162"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C22" s="162"/>
+      <c r="C22" s="163"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="12" t="s">
@@ -19436,32 +19953,32 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="164" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="164"/>
-      <c r="D4" s="163" t="s">
+      <c r="C4" s="165"/>
+      <c r="D4" s="164" t="s">
         <v>277</v>
       </c>
-      <c r="E4" s="164"/>
-      <c r="F4" s="165" t="s">
+      <c r="E4" s="165"/>
+      <c r="F4" s="166" t="s">
         <v>278</v>
       </c>
-      <c r="G4" s="164"/>
+      <c r="G4" s="165"/>
     </row>
     <row r="5" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="166" t="s">
+      <c r="B5" s="167" t="s">
         <v>279</v>
       </c>
-      <c r="C5" s="164"/>
-      <c r="D5" s="166" t="s">
+      <c r="C5" s="165"/>
+      <c r="D5" s="167" t="s">
         <v>280</v>
       </c>
-      <c r="E5" s="164"/>
-      <c r="F5" s="167" t="s">
+      <c r="E5" s="165"/>
+      <c r="F5" s="168" t="s">
         <v>281</v>
       </c>
-      <c r="G5" s="164"/>
+      <c r="G5" s="165"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
@@ -20841,18 +21358,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="152" t="s">
         <v>337</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
-      <c r="K2" s="151"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
@@ -22039,7 +22556,7 @@
   </sheetPr>
   <dimension ref="A3:S67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
@@ -22081,22 +22598,22 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="152" t="s">
+      <c r="E4" s="157" t="s">
         <v>487</v>
       </c>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
-      <c r="J4" s="153"/>
-      <c r="K4" s="153"/>
-      <c r="L4" s="153"/>
-      <c r="M4" s="153"/>
-      <c r="N4" s="153"/>
-      <c r="O4" s="153"/>
-      <c r="P4" s="153"/>
-      <c r="Q4" s="153"/>
-      <c r="R4" s="153"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="158"/>
+      <c r="J4" s="158"/>
+      <c r="K4" s="158"/>
+      <c r="L4" s="158"/>
+      <c r="M4" s="158"/>
+      <c r="N4" s="158"/>
+      <c r="O4" s="158"/>
+      <c r="P4" s="158"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="158"/>
       <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -22106,34 +22623,34 @@
       <c r="D5" s="126" t="s">
         <v>382</v>
       </c>
-      <c r="E5" s="154" t="s">
+      <c r="E5" s="159" t="s">
         <v>517</v>
       </c>
-      <c r="F5" s="155"/>
-      <c r="G5" s="154" t="s">
+      <c r="F5" s="160"/>
+      <c r="G5" s="159" t="s">
         <v>518</v>
       </c>
-      <c r="H5" s="155"/>
-      <c r="I5" s="154" t="s">
+      <c r="H5" s="160"/>
+      <c r="I5" s="159" t="s">
         <v>519</v>
       </c>
-      <c r="J5" s="155"/>
-      <c r="K5" s="154" t="s">
+      <c r="J5" s="160"/>
+      <c r="K5" s="159" t="s">
         <v>520</v>
       </c>
-      <c r="L5" s="155"/>
-      <c r="M5" s="154" t="s">
+      <c r="L5" s="160"/>
+      <c r="M5" s="159" t="s">
         <v>521</v>
       </c>
-      <c r="N5" s="155"/>
-      <c r="O5" s="154" t="s">
+      <c r="N5" s="160"/>
+      <c r="O5" s="159" t="s">
         <v>522</v>
       </c>
-      <c r="P5" s="155"/>
-      <c r="Q5" s="154" t="s">
+      <c r="P5" s="160"/>
+      <c r="Q5" s="159" t="s">
         <v>523</v>
       </c>
-      <c r="R5" s="155"/>
+      <c r="R5" s="160"/>
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25015,34 +25532,34 @@
       <c r="D64" s="131" t="s">
         <v>545</v>
       </c>
-      <c r="E64" s="158">
+      <c r="E64" s="155">
         <v>27.21</v>
       </c>
-      <c r="F64" s="157"/>
-      <c r="G64" s="159">
+      <c r="F64" s="154"/>
+      <c r="G64" s="156">
         <v>41.14</v>
       </c>
-      <c r="H64" s="157"/>
-      <c r="I64" s="156">
+      <c r="H64" s="154"/>
+      <c r="I64" s="153">
         <v>42.61</v>
       </c>
-      <c r="J64" s="157"/>
-      <c r="K64" s="156">
+      <c r="J64" s="154"/>
+      <c r="K64" s="153">
         <v>45.37</v>
       </c>
-      <c r="L64" s="157"/>
-      <c r="M64" s="156">
+      <c r="L64" s="154"/>
+      <c r="M64" s="153">
         <v>49.6</v>
       </c>
-      <c r="N64" s="157"/>
-      <c r="O64" s="156">
+      <c r="N64" s="154"/>
+      <c r="O64" s="153">
         <v>46.93</v>
       </c>
-      <c r="P64" s="157"/>
-      <c r="Q64" s="156">
+      <c r="P64" s="154"/>
+      <c r="Q64" s="153">
         <v>48.15</v>
       </c>
-      <c r="R64" s="157"/>
+      <c r="R64" s="154"/>
     </row>
     <row r="65" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
@@ -25051,34 +25568,34 @@
       <c r="D65" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="E65" s="158">
+      <c r="E65" s="155">
         <v>48483</v>
       </c>
-      <c r="F65" s="157"/>
-      <c r="G65" s="158">
+      <c r="F65" s="154"/>
+      <c r="G65" s="155">
         <v>17492</v>
       </c>
-      <c r="H65" s="157"/>
-      <c r="I65" s="158">
+      <c r="H65" s="154"/>
+      <c r="I65" s="155">
         <v>17492</v>
       </c>
-      <c r="J65" s="157"/>
-      <c r="K65" s="158">
+      <c r="J65" s="154"/>
+      <c r="K65" s="155">
         <v>17492</v>
       </c>
-      <c r="L65" s="157"/>
-      <c r="M65" s="156">
+      <c r="L65" s="154"/>
+      <c r="M65" s="153">
         <v>15660</v>
       </c>
-      <c r="N65" s="157"/>
-      <c r="O65" s="156">
+      <c r="N65" s="154"/>
+      <c r="O65" s="153">
         <v>11944</v>
       </c>
-      <c r="P65" s="157"/>
-      <c r="Q65" s="156">
+      <c r="P65" s="154"/>
+      <c r="Q65" s="153">
         <v>15422</v>
       </c>
-      <c r="R65" s="157"/>
+      <c r="R65" s="154"/>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
@@ -25126,6 +25643,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="Q64:R64"/>
     <mergeCell ref="E65:F65"/>
     <mergeCell ref="G65:H65"/>
@@ -25140,14 +25665,6 @@
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="M64:N64"/>
     <mergeCell ref="O64:P64"/>
-    <mergeCell ref="E4:R4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="portrait" r:id="rId1"/>
@@ -25173,17 +25690,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="152" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="151"/>
-      <c r="D4" s="151"/>
-      <c r="E4" s="151"/>
-      <c r="F4" s="151"/>
-      <c r="G4" s="151"/>
-      <c r="H4" s="151"/>
-      <c r="I4" s="151"/>
-      <c r="J4" s="151"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
     </row>
     <row r="6" spans="2:13" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -25800,7 +26317,7 @@
       <c r="B15" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="C15" s="160" t="s">
+      <c r="C15" s="161" t="s">
         <v>173</v>
       </c>
     </row>
@@ -25808,43 +26325,43 @@
       <c r="B16" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="C16" s="161"/>
+      <c r="C16" s="162"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="161"/>
+      <c r="C17" s="162"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C18" s="161"/>
+      <c r="C18" s="162"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="C19" s="161"/>
+      <c r="C19" s="162"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="C20" s="161"/>
+      <c r="C20" s="162"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C21" s="161"/>
+      <c r="C21" s="162"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C22" s="162"/>
+      <c r="C22" s="163"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="12" t="s">
@@ -26424,32 +26941,32 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="164" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="164"/>
-      <c r="D4" s="163" t="s">
+      <c r="C4" s="165"/>
+      <c r="D4" s="164" t="s">
         <v>277</v>
       </c>
-      <c r="E4" s="164"/>
-      <c r="F4" s="165" t="s">
+      <c r="E4" s="165"/>
+      <c r="F4" s="166" t="s">
         <v>278</v>
       </c>
-      <c r="G4" s="164"/>
+      <c r="G4" s="165"/>
     </row>
     <row r="5" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="166" t="s">
+      <c r="B5" s="167" t="s">
         <v>279</v>
       </c>
-      <c r="C5" s="164"/>
-      <c r="D5" s="166" t="s">
+      <c r="C5" s="165"/>
+      <c r="D5" s="167" t="s">
         <v>280</v>
       </c>
-      <c r="E5" s="164"/>
-      <c r="F5" s="167" t="s">
+      <c r="E5" s="165"/>
+      <c r="F5" s="168" t="s">
         <v>281</v>
       </c>
-      <c r="G5" s="164"/>
+      <c r="G5" s="165"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">

</xml_diff>

<commit_message>
Changes in tables (latex), means table, R files
</commit_message>
<xml_diff>
--- a/Excel/MASTER_VARIABLES_REGRESSIONS.xlsx
+++ b/Excel/MASTER_VARIABLES_REGRESSIONS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="966" firstSheet="10" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="966" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="20" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3165" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3166" uniqueCount="601">
   <si>
     <t>Non rotated part</t>
   </si>
@@ -2216,16 +2216,20 @@
   <si>
     <t xml:space="preserve">Math Reading Science - mean difference ranked </t>
   </si>
+  <si>
+    <t>AGE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="\(0.00\)"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -2817,7 +2821,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3021,6 +3025,18 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3032,18 +3048,6 @@
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3071,6 +3075,10 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7417,22 +7425,22 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="157" t="s">
+      <c r="E4" s="153" t="s">
         <v>488</v>
       </c>
-      <c r="F4" s="158"/>
-      <c r="G4" s="158"/>
-      <c r="H4" s="158"/>
-      <c r="I4" s="158"/>
-      <c r="J4" s="158"/>
-      <c r="K4" s="158"/>
-      <c r="L4" s="158"/>
-      <c r="M4" s="158"/>
-      <c r="N4" s="158"/>
-      <c r="O4" s="158"/>
-      <c r="P4" s="158"/>
-      <c r="Q4" s="158"/>
-      <c r="R4" s="158"/>
+      <c r="F4" s="154"/>
+      <c r="G4" s="154"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
+      <c r="K4" s="154"/>
+      <c r="L4" s="154"/>
+      <c r="M4" s="154"/>
+      <c r="N4" s="154"/>
+      <c r="O4" s="154"/>
+      <c r="P4" s="154"/>
+      <c r="Q4" s="154"/>
+      <c r="R4" s="154"/>
       <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -7442,34 +7450,34 @@
       <c r="D5" s="126" t="s">
         <v>382</v>
       </c>
-      <c r="E5" s="159" t="s">
+      <c r="E5" s="155" t="s">
         <v>517</v>
       </c>
-      <c r="F5" s="160"/>
-      <c r="G5" s="159" t="s">
+      <c r="F5" s="156"/>
+      <c r="G5" s="155" t="s">
         <v>518</v>
       </c>
-      <c r="H5" s="160"/>
-      <c r="I5" s="159" t="s">
+      <c r="H5" s="156"/>
+      <c r="I5" s="155" t="s">
         <v>519</v>
       </c>
-      <c r="J5" s="160"/>
-      <c r="K5" s="159" t="s">
+      <c r="J5" s="156"/>
+      <c r="K5" s="155" t="s">
         <v>520</v>
       </c>
-      <c r="L5" s="160"/>
-      <c r="M5" s="159" t="s">
+      <c r="L5" s="156"/>
+      <c r="M5" s="155" t="s">
         <v>521</v>
       </c>
-      <c r="N5" s="160"/>
-      <c r="O5" s="159" t="s">
+      <c r="N5" s="156"/>
+      <c r="O5" s="155" t="s">
         <v>522</v>
       </c>
-      <c r="P5" s="160"/>
-      <c r="Q5" s="159" t="s">
+      <c r="P5" s="156"/>
+      <c r="Q5" s="155" t="s">
         <v>523</v>
       </c>
-      <c r="R5" s="160"/>
+      <c r="R5" s="156"/>
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9601,34 +9609,34 @@
       <c r="D49" s="131" t="s">
         <v>545</v>
       </c>
-      <c r="E49" s="155">
+      <c r="E49" s="159">
         <v>19.61</v>
       </c>
-      <c r="F49" s="153"/>
-      <c r="G49" s="156">
+      <c r="F49" s="157"/>
+      <c r="G49" s="160">
         <v>38.72</v>
       </c>
-      <c r="H49" s="153"/>
-      <c r="I49" s="153">
+      <c r="H49" s="157"/>
+      <c r="I49" s="157">
         <v>39.26</v>
       </c>
-      <c r="J49" s="153"/>
-      <c r="K49" s="153">
+      <c r="J49" s="157"/>
+      <c r="K49" s="157">
         <v>43.09</v>
       </c>
-      <c r="L49" s="153"/>
-      <c r="M49" s="153">
+      <c r="L49" s="157"/>
+      <c r="M49" s="157">
         <v>42.69</v>
       </c>
-      <c r="N49" s="153"/>
-      <c r="O49" s="153">
+      <c r="N49" s="157"/>
+      <c r="O49" s="157">
         <v>39.82</v>
       </c>
-      <c r="P49" s="153"/>
-      <c r="Q49" s="153">
+      <c r="P49" s="157"/>
+      <c r="Q49" s="157">
         <v>43.62</v>
       </c>
-      <c r="R49" s="153"/>
+      <c r="R49" s="157"/>
     </row>
     <row r="50" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
@@ -9637,34 +9645,34 @@
       <c r="D50" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="E50" s="155">
+      <c r="E50" s="159">
         <v>48483</v>
       </c>
-      <c r="F50" s="153"/>
-      <c r="G50" s="155">
+      <c r="F50" s="157"/>
+      <c r="G50" s="159">
         <v>18474</v>
       </c>
-      <c r="H50" s="153"/>
-      <c r="I50" s="155">
+      <c r="H50" s="157"/>
+      <c r="I50" s="159">
         <v>18474</v>
       </c>
-      <c r="J50" s="153"/>
-      <c r="K50" s="155">
+      <c r="J50" s="157"/>
+      <c r="K50" s="159">
         <v>18474</v>
       </c>
-      <c r="L50" s="153"/>
-      <c r="M50" s="153">
+      <c r="L50" s="157"/>
+      <c r="M50" s="157">
         <v>17506</v>
       </c>
-      <c r="N50" s="153"/>
-      <c r="O50" s="153">
+      <c r="N50" s="157"/>
+      <c r="O50" s="157">
         <v>11843</v>
       </c>
-      <c r="P50" s="153"/>
-      <c r="Q50" s="153">
+      <c r="P50" s="157"/>
+      <c r="Q50" s="157">
         <v>16829</v>
       </c>
-      <c r="R50" s="153"/>
+      <c r="R50" s="157"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
@@ -9712,14 +9720,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E4:R4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="Q49:R49"/>
     <mergeCell ref="E50:F50"/>
     <mergeCell ref="G50:H50"/>
@@ -9734,6 +9734,14 @@
     <mergeCell ref="K49:L49"/>
     <mergeCell ref="M49:N49"/>
     <mergeCell ref="O49:P49"/>
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14280,7 +14288,7 @@
   </sheetPr>
   <dimension ref="A3:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q50" sqref="D4:R50"/>
     </sheetView>
   </sheetViews>
@@ -14322,22 +14330,22 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="157" t="s">
+      <c r="E4" s="153" t="s">
         <v>489</v>
       </c>
-      <c r="F4" s="158"/>
-      <c r="G4" s="158"/>
-      <c r="H4" s="158"/>
-      <c r="I4" s="158"/>
-      <c r="J4" s="158"/>
-      <c r="K4" s="158"/>
-      <c r="L4" s="158"/>
-      <c r="M4" s="158"/>
-      <c r="N4" s="158"/>
-      <c r="O4" s="158"/>
-      <c r="P4" s="158"/>
-      <c r="Q4" s="158"/>
-      <c r="R4" s="158"/>
+      <c r="F4" s="154"/>
+      <c r="G4" s="154"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
+      <c r="K4" s="154"/>
+      <c r="L4" s="154"/>
+      <c r="M4" s="154"/>
+      <c r="N4" s="154"/>
+      <c r="O4" s="154"/>
+      <c r="P4" s="154"/>
+      <c r="Q4" s="154"/>
+      <c r="R4" s="154"/>
       <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -14347,34 +14355,34 @@
       <c r="D5" s="126" t="s">
         <v>382</v>
       </c>
-      <c r="E5" s="159" t="s">
+      <c r="E5" s="155" t="s">
         <v>517</v>
       </c>
-      <c r="F5" s="160"/>
-      <c r="G5" s="159" t="s">
+      <c r="F5" s="156"/>
+      <c r="G5" s="155" t="s">
         <v>518</v>
       </c>
-      <c r="H5" s="160"/>
-      <c r="I5" s="159" t="s">
+      <c r="H5" s="156"/>
+      <c r="I5" s="155" t="s">
         <v>519</v>
       </c>
-      <c r="J5" s="160"/>
-      <c r="K5" s="159" t="s">
+      <c r="J5" s="156"/>
+      <c r="K5" s="155" t="s">
         <v>520</v>
       </c>
-      <c r="L5" s="160"/>
-      <c r="M5" s="159" t="s">
+      <c r="L5" s="156"/>
+      <c r="M5" s="155" t="s">
         <v>521</v>
       </c>
-      <c r="N5" s="160"/>
-      <c r="O5" s="159" t="s">
+      <c r="N5" s="156"/>
+      <c r="O5" s="155" t="s">
         <v>522</v>
       </c>
-      <c r="P5" s="160"/>
-      <c r="Q5" s="159" t="s">
+      <c r="P5" s="156"/>
+      <c r="Q5" s="155" t="s">
         <v>523</v>
       </c>
-      <c r="R5" s="160"/>
+      <c r="R5" s="156"/>
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16506,34 +16514,34 @@
       <c r="D49" s="131" t="s">
         <v>545</v>
       </c>
-      <c r="E49" s="155">
+      <c r="E49" s="159">
         <v>30.75</v>
       </c>
-      <c r="F49" s="153"/>
-      <c r="G49" s="156">
+      <c r="F49" s="157"/>
+      <c r="G49" s="160">
         <v>44.59</v>
       </c>
-      <c r="H49" s="153"/>
-      <c r="I49" s="153">
+      <c r="H49" s="157"/>
+      <c r="I49" s="157">
         <v>45.04</v>
       </c>
-      <c r="J49" s="153"/>
-      <c r="K49" s="153">
+      <c r="J49" s="157"/>
+      <c r="K49" s="157">
         <v>48.32</v>
       </c>
-      <c r="L49" s="153"/>
-      <c r="M49" s="153">
+      <c r="L49" s="157"/>
+      <c r="M49" s="157">
         <v>47.61</v>
       </c>
-      <c r="N49" s="153"/>
-      <c r="O49" s="153">
+      <c r="N49" s="157"/>
+      <c r="O49" s="157">
         <v>45.52</v>
       </c>
-      <c r="P49" s="153"/>
-      <c r="Q49" s="153">
+      <c r="P49" s="157"/>
+      <c r="Q49" s="157">
         <v>49.19</v>
       </c>
-      <c r="R49" s="153"/>
+      <c r="R49" s="157"/>
     </row>
     <row r="50" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
@@ -16542,34 +16550,34 @@
       <c r="D50" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="E50" s="155">
+      <c r="E50" s="159">
         <v>48483</v>
       </c>
-      <c r="F50" s="153"/>
-      <c r="G50" s="155">
+      <c r="F50" s="157"/>
+      <c r="G50" s="159">
         <v>18474</v>
       </c>
-      <c r="H50" s="153"/>
-      <c r="I50" s="155">
+      <c r="H50" s="157"/>
+      <c r="I50" s="159">
         <v>18474</v>
       </c>
-      <c r="J50" s="153"/>
-      <c r="K50" s="155">
+      <c r="J50" s="157"/>
+      <c r="K50" s="159">
         <v>18474</v>
       </c>
-      <c r="L50" s="153"/>
-      <c r="M50" s="153">
+      <c r="L50" s="157"/>
+      <c r="M50" s="157">
         <v>17441</v>
       </c>
-      <c r="N50" s="153"/>
-      <c r="O50" s="153">
+      <c r="N50" s="157"/>
+      <c r="O50" s="157">
         <v>12670</v>
       </c>
-      <c r="P50" s="153"/>
-      <c r="Q50" s="153">
+      <c r="P50" s="157"/>
+      <c r="Q50" s="157">
         <v>16764</v>
       </c>
-      <c r="R50" s="153"/>
+      <c r="R50" s="157"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
@@ -16617,6 +16625,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="Q49:R49"/>
     <mergeCell ref="E50:F50"/>
     <mergeCell ref="G50:H50"/>
@@ -16631,14 +16647,6 @@
     <mergeCell ref="K49:L49"/>
     <mergeCell ref="M49:N49"/>
     <mergeCell ref="O49:P49"/>
-    <mergeCell ref="E4:R4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="portrait" r:id="rId1"/>
@@ -16652,8 +16660,8 @@
   </sheetPr>
   <dimension ref="A2:T130"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19235,19 +19243,19 @@
         <v>17.923999999999999</v>
       </c>
       <c r="H67" s="1">
-        <f t="shared" ref="H67:H125" si="4">D67-C67</f>
+        <f t="shared" ref="H67:H126" si="4">D67-C67</f>
         <v>-0.16188846599999995</v>
       </c>
       <c r="I67" s="1">
-        <f t="shared" ref="I67:I125" si="5">C67</f>
+        <f t="shared" ref="I67:I126" si="5">C67</f>
         <v>0.52493396299999995</v>
       </c>
       <c r="J67" s="53">
-        <f t="shared" ref="J67:J125" si="6">H67/I67</f>
+        <f t="shared" ref="J67:J126" si="6">H67/I67</f>
         <v>-0.30839777459779255</v>
       </c>
       <c r="K67" s="53">
-        <f t="shared" ref="K67:K125" si="7">ABS(J67)</f>
+        <f t="shared" ref="K67:K126" si="7">ABS(J67)</f>
         <v>0.30839777459779255</v>
       </c>
       <c r="O67" s="139"/>
@@ -21180,60 +21188,93 @@
         <f t="shared" si="5"/>
         <v>0.82703777300000003</v>
       </c>
-      <c r="J124" s="53">
+      <c r="J124" s="72">
         <f t="shared" si="6"/>
         <v>3.5668709414557942E-3</v>
       </c>
-      <c r="K124" s="53">
+      <c r="K124" s="72">
         <f t="shared" si="7"/>
         <v>3.5668709414557942E-3</v>
       </c>
       <c r="O124" s="139"/>
     </row>
-    <row r="125" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B125" s="146" t="s">
-        <v>46</v>
+    <row r="125" spans="2:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B125" s="1" t="s">
+        <v>600</v>
       </c>
       <c r="C125" s="1">
-        <v>0.87556086300000002</v>
+        <v>15.8211743248864</v>
       </c>
       <c r="D125" s="1">
-        <v>0.87747514900000001</v>
+        <v>15.7692499481082</v>
       </c>
       <c r="E125" s="140">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="F125" s="146">
-        <v>-0.45800000000000002</v>
-      </c>
+        <v>4.5291810812727102E-32</v>
+      </c>
+      <c r="F125" s="140">
+        <v>11.855916328726201</v>
+      </c>
+      <c r="G125" s="1"/>
       <c r="H125" s="1">
         <f t="shared" si="4"/>
-        <v>1.9142859999999873E-3</v>
+        <v>-5.1924376778199388E-2</v>
       </c>
       <c r="I125" s="1">
         <f t="shared" si="5"/>
+        <v>15.8211743248864</v>
+      </c>
+      <c r="J125" s="170">
+        <f t="shared" si="6"/>
+        <v>-3.281954658480904E-3</v>
+      </c>
+      <c r="K125" s="170">
+        <f t="shared" si="7"/>
+        <v>3.281954658480904E-3</v>
+      </c>
+      <c r="O125" s="171"/>
+    </row>
+    <row r="126" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B126" s="146" t="s">
+        <v>46</v>
+      </c>
+      <c r="C126" s="1">
         <v>0.87556086300000002</v>
       </c>
-      <c r="J125" s="53">
+      <c r="D126" s="1">
+        <v>0.87747514900000001</v>
+      </c>
+      <c r="E126" s="140">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="F126" s="146">
+        <v>-0.45800000000000002</v>
+      </c>
+      <c r="H126" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9142859999999873E-3</v>
+      </c>
+      <c r="I126" s="1">
+        <f t="shared" si="5"/>
+        <v>0.87556086300000002</v>
+      </c>
+      <c r="J126" s="72">
         <f t="shared" si="6"/>
         <v>2.1863540056380835E-3</v>
       </c>
-      <c r="K125" s="53">
+      <c r="K126" s="72">
         <f t="shared" si="7"/>
         <v>2.1863540056380835E-3</v>
       </c>
-      <c r="O125" s="139"/>
-    </row>
-    <row r="126" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="J126" s="53"/>
-      <c r="K126" s="53"/>
+      <c r="O126" s="139"/>
     </row>
     <row r="127" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D127" s="147"/>
-      <c r="O127" s="1"/>
+      <c r="J127" s="53"/>
+      <c r="K127" s="53"/>
     </row>
     <row r="128" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="J128" s="147"/>
+      <c r="D128" s="147"/>
+      <c r="J128" s="53"/>
+      <c r="K128" s="53"/>
       <c r="O128" s="1"/>
     </row>
     <row r="129" spans="10:15" x14ac:dyDescent="0.2">
@@ -24971,22 +25012,22 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="157" t="s">
+      <c r="E4" s="153" t="s">
         <v>487</v>
       </c>
-      <c r="F4" s="158"/>
-      <c r="G4" s="158"/>
-      <c r="H4" s="158"/>
-      <c r="I4" s="158"/>
-      <c r="J4" s="158"/>
-      <c r="K4" s="158"/>
-      <c r="L4" s="158"/>
-      <c r="M4" s="158"/>
-      <c r="N4" s="158"/>
-      <c r="O4" s="158"/>
-      <c r="P4" s="158"/>
-      <c r="Q4" s="158"/>
-      <c r="R4" s="158"/>
+      <c r="F4" s="154"/>
+      <c r="G4" s="154"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
+      <c r="K4" s="154"/>
+      <c r="L4" s="154"/>
+      <c r="M4" s="154"/>
+      <c r="N4" s="154"/>
+      <c r="O4" s="154"/>
+      <c r="P4" s="154"/>
+      <c r="Q4" s="154"/>
+      <c r="R4" s="154"/>
       <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -24996,34 +25037,34 @@
       <c r="D5" s="126" t="s">
         <v>382</v>
       </c>
-      <c r="E5" s="159" t="s">
+      <c r="E5" s="155" t="s">
         <v>517</v>
       </c>
-      <c r="F5" s="160"/>
-      <c r="G5" s="159" t="s">
+      <c r="F5" s="156"/>
+      <c r="G5" s="155" t="s">
         <v>518</v>
       </c>
-      <c r="H5" s="160"/>
-      <c r="I5" s="159" t="s">
+      <c r="H5" s="156"/>
+      <c r="I5" s="155" t="s">
         <v>519</v>
       </c>
-      <c r="J5" s="160"/>
-      <c r="K5" s="159" t="s">
+      <c r="J5" s="156"/>
+      <c r="K5" s="155" t="s">
         <v>520</v>
       </c>
-      <c r="L5" s="160"/>
-      <c r="M5" s="159" t="s">
+      <c r="L5" s="156"/>
+      <c r="M5" s="155" t="s">
         <v>521</v>
       </c>
-      <c r="N5" s="160"/>
-      <c r="O5" s="159" t="s">
+      <c r="N5" s="156"/>
+      <c r="O5" s="155" t="s">
         <v>522</v>
       </c>
-      <c r="P5" s="160"/>
-      <c r="Q5" s="159" t="s">
+      <c r="P5" s="156"/>
+      <c r="Q5" s="155" t="s">
         <v>523</v>
       </c>
-      <c r="R5" s="160"/>
+      <c r="R5" s="156"/>
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27905,34 +27946,34 @@
       <c r="D64" s="131" t="s">
         <v>545</v>
       </c>
-      <c r="E64" s="155">
+      <c r="E64" s="159">
         <v>27.21</v>
       </c>
-      <c r="F64" s="154"/>
-      <c r="G64" s="156">
+      <c r="F64" s="158"/>
+      <c r="G64" s="160">
         <v>41.14</v>
       </c>
-      <c r="H64" s="154"/>
-      <c r="I64" s="153">
+      <c r="H64" s="158"/>
+      <c r="I64" s="157">
         <v>42.61</v>
       </c>
-      <c r="J64" s="154"/>
-      <c r="K64" s="153">
+      <c r="J64" s="158"/>
+      <c r="K64" s="157">
         <v>45.37</v>
       </c>
-      <c r="L64" s="154"/>
-      <c r="M64" s="153">
+      <c r="L64" s="158"/>
+      <c r="M64" s="157">
         <v>49.6</v>
       </c>
-      <c r="N64" s="154"/>
-      <c r="O64" s="153">
+      <c r="N64" s="158"/>
+      <c r="O64" s="157">
         <v>46.93</v>
       </c>
-      <c r="P64" s="154"/>
-      <c r="Q64" s="153">
+      <c r="P64" s="158"/>
+      <c r="Q64" s="157">
         <v>48.15</v>
       </c>
-      <c r="R64" s="154"/>
+      <c r="R64" s="158"/>
     </row>
     <row r="65" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
@@ -27941,34 +27982,34 @@
       <c r="D65" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="E65" s="155">
+      <c r="E65" s="159">
         <v>48483</v>
       </c>
-      <c r="F65" s="154"/>
-      <c r="G65" s="155">
+      <c r="F65" s="158"/>
+      <c r="G65" s="159">
         <v>17492</v>
       </c>
-      <c r="H65" s="154"/>
-      <c r="I65" s="155">
+      <c r="H65" s="158"/>
+      <c r="I65" s="159">
         <v>17492</v>
       </c>
-      <c r="J65" s="154"/>
-      <c r="K65" s="155">
+      <c r="J65" s="158"/>
+      <c r="K65" s="159">
         <v>17492</v>
       </c>
-      <c r="L65" s="154"/>
-      <c r="M65" s="153">
+      <c r="L65" s="158"/>
+      <c r="M65" s="157">
         <v>15660</v>
       </c>
-      <c r="N65" s="154"/>
-      <c r="O65" s="153">
+      <c r="N65" s="158"/>
+      <c r="O65" s="157">
         <v>11944</v>
       </c>
-      <c r="P65" s="154"/>
-      <c r="Q65" s="153">
+      <c r="P65" s="158"/>
+      <c r="Q65" s="157">
         <v>15422</v>
       </c>
-      <c r="R65" s="154"/>
+      <c r="R65" s="158"/>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
@@ -28016,14 +28057,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E4:R4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="Q64:R64"/>
     <mergeCell ref="E65:F65"/>
     <mergeCell ref="G65:H65"/>
@@ -28038,6 +28071,14 @@
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="M64:N64"/>
     <mergeCell ref="O64:P64"/>
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Master file excel - minor changes
</commit_message>
<xml_diff>
--- a/Excel/MASTER_VARIABLES_REGRESSIONS.xlsx
+++ b/Excel/MASTER_VARIABLES_REGRESSIONS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="966" firstSheet="13" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="966"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="20" r:id="rId1"/>
@@ -3068,6 +3068,12 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3081,12 +3087,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -4559,7 +4559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:M40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
@@ -5699,7 +5699,7 @@
     <mergeCell ref="F5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="76" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="99" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8135,18 +8135,18 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="155" t="s">
+      <c r="E4" s="157" t="s">
         <v>484</v>
       </c>
-      <c r="F4" s="156"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="156"/>
-      <c r="I4" s="156"/>
-      <c r="J4" s="156"/>
-      <c r="K4" s="156"/>
-      <c r="L4" s="156"/>
-      <c r="M4" s="156"/>
-      <c r="N4" s="156"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="158"/>
+      <c r="J4" s="158"/>
+      <c r="K4" s="158"/>
+      <c r="L4" s="158"/>
+      <c r="M4" s="158"/>
+      <c r="N4" s="158"/>
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -8156,26 +8156,26 @@
       <c r="D5" s="126" t="s">
         <v>382</v>
       </c>
-      <c r="E5" s="157" t="s">
+      <c r="E5" s="159" t="s">
         <v>513</v>
       </c>
-      <c r="F5" s="158"/>
-      <c r="G5" s="157" t="s">
+      <c r="F5" s="160"/>
+      <c r="G5" s="159" t="s">
         <v>514</v>
       </c>
-      <c r="H5" s="158"/>
-      <c r="I5" s="157" t="s">
+      <c r="H5" s="160"/>
+      <c r="I5" s="159" t="s">
         <v>515</v>
       </c>
-      <c r="J5" s="158"/>
-      <c r="K5" s="157" t="s">
+      <c r="J5" s="160"/>
+      <c r="K5" s="159" t="s">
         <v>516</v>
       </c>
-      <c r="L5" s="158"/>
-      <c r="M5" s="157" t="s">
+      <c r="L5" s="160"/>
+      <c r="M5" s="159" t="s">
         <v>517</v>
       </c>
-      <c r="N5" s="158"/>
+      <c r="N5" s="160"/>
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9533,26 +9533,26 @@
       <c r="D42" s="131" t="s">
         <v>541</v>
       </c>
-      <c r="E42" s="161">
+      <c r="E42" s="155">
         <v>19.61</v>
       </c>
-      <c r="F42" s="159"/>
-      <c r="G42" s="161">
+      <c r="F42" s="161"/>
+      <c r="G42" s="155">
         <v>34.5</v>
       </c>
-      <c r="H42" s="159"/>
-      <c r="I42" s="161">
+      <c r="H42" s="161"/>
+      <c r="I42" s="155">
         <v>36.450000000000003</v>
       </c>
-      <c r="J42" s="159"/>
-      <c r="K42" s="161">
+      <c r="J42" s="161"/>
+      <c r="K42" s="155">
         <v>39.630000000000003</v>
       </c>
-      <c r="L42" s="159"/>
-      <c r="M42" s="161">
+      <c r="L42" s="161"/>
+      <c r="M42" s="155">
         <v>41.84</v>
       </c>
-      <c r="N42" s="159"/>
+      <c r="N42" s="161"/>
     </row>
     <row r="43" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
@@ -9561,26 +9561,26 @@
       <c r="D43" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="E43" s="161">
+      <c r="E43" s="155">
         <v>48483</v>
       </c>
-      <c r="F43" s="159"/>
-      <c r="G43" s="161">
+      <c r="F43" s="161"/>
+      <c r="G43" s="155">
         <v>46267</v>
       </c>
-      <c r="H43" s="159"/>
-      <c r="I43" s="161">
+      <c r="H43" s="161"/>
+      <c r="I43" s="155">
         <v>44046</v>
       </c>
-      <c r="J43" s="159"/>
-      <c r="K43" s="161">
+      <c r="J43" s="161"/>
+      <c r="K43" s="155">
         <v>35442</v>
       </c>
-      <c r="L43" s="159"/>
-      <c r="M43" s="161">
+      <c r="L43" s="161"/>
+      <c r="M43" s="155">
         <v>27331</v>
       </c>
-      <c r="N43" s="159"/>
+      <c r="N43" s="161"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
@@ -9593,8 +9593,8 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
-      <c r="K44" s="161"/>
-      <c r="L44" s="159"/>
+      <c r="K44" s="155"/>
+      <c r="L44" s="161"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
@@ -9620,23 +9620,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="E4:N4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="M43:N43"/>
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="I42:J42"/>
     <mergeCell ref="K42:L42"/>
     <mergeCell ref="M42:N42"/>
-    <mergeCell ref="E4:N4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K43:L43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9689,22 +9689,22 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="155" t="s">
+      <c r="E4" s="157" t="s">
         <v>484</v>
       </c>
-      <c r="F4" s="156"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="156"/>
-      <c r="I4" s="156"/>
-      <c r="J4" s="156"/>
-      <c r="K4" s="156"/>
-      <c r="L4" s="156"/>
-      <c r="M4" s="156"/>
-      <c r="N4" s="156"/>
-      <c r="O4" s="156"/>
-      <c r="P4" s="156"/>
-      <c r="Q4" s="156"/>
-      <c r="R4" s="156"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="158"/>
+      <c r="J4" s="158"/>
+      <c r="K4" s="158"/>
+      <c r="L4" s="158"/>
+      <c r="M4" s="158"/>
+      <c r="N4" s="158"/>
+      <c r="O4" s="158"/>
+      <c r="P4" s="158"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="158"/>
       <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -9714,34 +9714,34 @@
       <c r="D5" s="126" t="s">
         <v>382</v>
       </c>
-      <c r="E5" s="157" t="s">
+      <c r="E5" s="159" t="s">
         <v>513</v>
       </c>
-      <c r="F5" s="158"/>
-      <c r="G5" s="157" t="s">
+      <c r="F5" s="160"/>
+      <c r="G5" s="159" t="s">
         <v>514</v>
       </c>
-      <c r="H5" s="158"/>
-      <c r="I5" s="157" t="s">
+      <c r="H5" s="160"/>
+      <c r="I5" s="159" t="s">
         <v>515</v>
       </c>
-      <c r="J5" s="158"/>
-      <c r="K5" s="157" t="s">
+      <c r="J5" s="160"/>
+      <c r="K5" s="159" t="s">
         <v>516</v>
       </c>
-      <c r="L5" s="158"/>
-      <c r="M5" s="157" t="s">
+      <c r="L5" s="160"/>
+      <c r="M5" s="159" t="s">
         <v>517</v>
       </c>
-      <c r="N5" s="158"/>
-      <c r="O5" s="157" t="s">
+      <c r="N5" s="160"/>
+      <c r="O5" s="159" t="s">
         <v>518</v>
       </c>
-      <c r="P5" s="158"/>
-      <c r="Q5" s="157" t="s">
+      <c r="P5" s="160"/>
+      <c r="Q5" s="159" t="s">
         <v>519</v>
       </c>
-      <c r="R5" s="158"/>
+      <c r="R5" s="160"/>
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11873,34 +11873,34 @@
       <c r="D49" s="131" t="s">
         <v>541</v>
       </c>
-      <c r="E49" s="161">
+      <c r="E49" s="155">
         <v>19.61</v>
       </c>
-      <c r="F49" s="159"/>
+      <c r="F49" s="161"/>
       <c r="G49" s="162">
         <v>38.72</v>
       </c>
-      <c r="H49" s="159"/>
-      <c r="I49" s="159">
+      <c r="H49" s="161"/>
+      <c r="I49" s="161">
         <v>39.26</v>
       </c>
-      <c r="J49" s="159"/>
-      <c r="K49" s="159">
+      <c r="J49" s="161"/>
+      <c r="K49" s="161">
         <v>43.09</v>
       </c>
-      <c r="L49" s="159"/>
-      <c r="M49" s="159">
+      <c r="L49" s="161"/>
+      <c r="M49" s="161">
         <v>42.69</v>
       </c>
-      <c r="N49" s="159"/>
-      <c r="O49" s="159">
+      <c r="N49" s="161"/>
+      <c r="O49" s="161">
         <v>39.82</v>
       </c>
-      <c r="P49" s="159"/>
-      <c r="Q49" s="159">
+      <c r="P49" s="161"/>
+      <c r="Q49" s="161">
         <v>43.62</v>
       </c>
-      <c r="R49" s="159"/>
+      <c r="R49" s="161"/>
     </row>
     <row r="50" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
@@ -11909,34 +11909,34 @@
       <c r="D50" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="E50" s="161">
+      <c r="E50" s="155">
         <v>48483</v>
       </c>
-      <c r="F50" s="159"/>
-      <c r="G50" s="161">
+      <c r="F50" s="161"/>
+      <c r="G50" s="155">
         <v>18474</v>
       </c>
-      <c r="H50" s="159"/>
-      <c r="I50" s="161">
+      <c r="H50" s="161"/>
+      <c r="I50" s="155">
         <v>18474</v>
       </c>
-      <c r="J50" s="159"/>
-      <c r="K50" s="161">
+      <c r="J50" s="161"/>
+      <c r="K50" s="155">
         <v>18474</v>
       </c>
-      <c r="L50" s="159"/>
-      <c r="M50" s="159">
+      <c r="L50" s="161"/>
+      <c r="M50" s="161">
         <v>17506</v>
       </c>
-      <c r="N50" s="159"/>
-      <c r="O50" s="159">
+      <c r="N50" s="161"/>
+      <c r="O50" s="161">
         <v>11843</v>
       </c>
-      <c r="P50" s="159"/>
-      <c r="Q50" s="159">
+      <c r="P50" s="161"/>
+      <c r="Q50" s="161">
         <v>16829</v>
       </c>
-      <c r="R50" s="159"/>
+      <c r="R50" s="161"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
@@ -11984,14 +11984,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E4:R4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="Q49:R49"/>
     <mergeCell ref="E50:F50"/>
     <mergeCell ref="G50:H50"/>
@@ -12006,6 +11998,14 @@
     <mergeCell ref="K49:L49"/>
     <mergeCell ref="M49:N49"/>
     <mergeCell ref="O49:P49"/>
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14779,8 +14779,8 @@
   </sheetPr>
   <dimension ref="A2:T130"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M9" activeCellId="1" sqref="B12:M12 B9:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21256,7 +21256,7 @@
   </sheetPr>
   <dimension ref="A3:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
@@ -21294,18 +21294,18 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="155" t="s">
+      <c r="E4" s="157" t="s">
         <v>485</v>
       </c>
-      <c r="F4" s="156"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="156"/>
-      <c r="I4" s="156"/>
-      <c r="J4" s="156"/>
-      <c r="K4" s="156"/>
-      <c r="L4" s="156"/>
-      <c r="M4" s="156"/>
-      <c r="N4" s="156"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="158"/>
+      <c r="J4" s="158"/>
+      <c r="K4" s="158"/>
+      <c r="L4" s="158"/>
+      <c r="M4" s="158"/>
+      <c r="N4" s="158"/>
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -21315,26 +21315,26 @@
       <c r="D5" s="126" t="s">
         <v>382</v>
       </c>
-      <c r="E5" s="157" t="s">
+      <c r="E5" s="159" t="s">
         <v>513</v>
       </c>
-      <c r="F5" s="158"/>
-      <c r="G5" s="157" t="s">
+      <c r="F5" s="160"/>
+      <c r="G5" s="159" t="s">
         <v>514</v>
       </c>
-      <c r="H5" s="158"/>
-      <c r="I5" s="157" t="s">
+      <c r="H5" s="160"/>
+      <c r="I5" s="159" t="s">
         <v>515</v>
       </c>
-      <c r="J5" s="158"/>
-      <c r="K5" s="157" t="s">
+      <c r="J5" s="160"/>
+      <c r="K5" s="159" t="s">
         <v>516</v>
       </c>
-      <c r="L5" s="158"/>
-      <c r="M5" s="157" t="s">
+      <c r="L5" s="160"/>
+      <c r="M5" s="159" t="s">
         <v>517</v>
       </c>
-      <c r="N5" s="158"/>
+      <c r="N5" s="160"/>
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -22730,26 +22730,26 @@
       <c r="D43" s="131" t="s">
         <v>541</v>
       </c>
-      <c r="E43" s="161">
+      <c r="E43" s="155">
         <v>30.75</v>
       </c>
-      <c r="F43" s="159"/>
-      <c r="G43" s="161">
+      <c r="F43" s="161"/>
+      <c r="G43" s="155">
         <v>41.14</v>
       </c>
-      <c r="H43" s="159"/>
-      <c r="I43" s="161">
+      <c r="H43" s="161"/>
+      <c r="I43" s="155">
         <v>43.35</v>
       </c>
-      <c r="J43" s="159"/>
-      <c r="K43" s="161">
+      <c r="J43" s="161"/>
+      <c r="K43" s="155">
         <v>46.11</v>
       </c>
-      <c r="L43" s="159"/>
-      <c r="M43" s="161">
+      <c r="L43" s="161"/>
+      <c r="M43" s="155">
         <v>47.35</v>
       </c>
-      <c r="N43" s="159"/>
+      <c r="N43" s="161"/>
     </row>
     <row r="44" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
@@ -22758,26 +22758,26 @@
       <c r="D44" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="E44" s="161">
+      <c r="E44" s="155">
         <v>48483</v>
       </c>
-      <c r="F44" s="159"/>
-      <c r="G44" s="161">
+      <c r="F44" s="161"/>
+      <c r="G44" s="155">
         <v>46267</v>
       </c>
-      <c r="H44" s="159"/>
-      <c r="I44" s="161">
+      <c r="H44" s="161"/>
+      <c r="I44" s="155">
         <v>44046</v>
       </c>
-      <c r="J44" s="159"/>
-      <c r="K44" s="161">
+      <c r="J44" s="161"/>
+      <c r="K44" s="155">
         <v>35302</v>
       </c>
-      <c r="L44" s="159"/>
-      <c r="M44" s="161">
+      <c r="L44" s="161"/>
+      <c r="M44" s="155">
         <v>27224</v>
       </c>
-      <c r="N44" s="159"/>
+      <c r="N44" s="161"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
@@ -22817,22 +22817,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
     <mergeCell ref="E4:N4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="portrait" r:id="rId1"/>
@@ -22888,22 +22888,22 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="155" t="s">
+      <c r="E4" s="157" t="s">
         <v>485</v>
       </c>
-      <c r="F4" s="156"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="156"/>
-      <c r="I4" s="156"/>
-      <c r="J4" s="156"/>
-      <c r="K4" s="156"/>
-      <c r="L4" s="156"/>
-      <c r="M4" s="156"/>
-      <c r="N4" s="156"/>
-      <c r="O4" s="156"/>
-      <c r="P4" s="156"/>
-      <c r="Q4" s="156"/>
-      <c r="R4" s="156"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="158"/>
+      <c r="J4" s="158"/>
+      <c r="K4" s="158"/>
+      <c r="L4" s="158"/>
+      <c r="M4" s="158"/>
+      <c r="N4" s="158"/>
+      <c r="O4" s="158"/>
+      <c r="P4" s="158"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="158"/>
       <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -22913,34 +22913,34 @@
       <c r="D5" s="126" t="s">
         <v>382</v>
       </c>
-      <c r="E5" s="157" t="s">
+      <c r="E5" s="159" t="s">
         <v>513</v>
       </c>
-      <c r="F5" s="158"/>
-      <c r="G5" s="157" t="s">
+      <c r="F5" s="160"/>
+      <c r="G5" s="159" t="s">
         <v>514</v>
       </c>
-      <c r="H5" s="158"/>
-      <c r="I5" s="157" t="s">
+      <c r="H5" s="160"/>
+      <c r="I5" s="159" t="s">
         <v>515</v>
       </c>
-      <c r="J5" s="158"/>
-      <c r="K5" s="157" t="s">
+      <c r="J5" s="160"/>
+      <c r="K5" s="159" t="s">
         <v>516</v>
       </c>
-      <c r="L5" s="158"/>
-      <c r="M5" s="157" t="s">
+      <c r="L5" s="160"/>
+      <c r="M5" s="159" t="s">
         <v>517</v>
       </c>
-      <c r="N5" s="158"/>
-      <c r="O5" s="157" t="s">
+      <c r="N5" s="160"/>
+      <c r="O5" s="159" t="s">
         <v>518</v>
       </c>
-      <c r="P5" s="158"/>
-      <c r="Q5" s="157" t="s">
+      <c r="P5" s="160"/>
+      <c r="Q5" s="159" t="s">
         <v>519</v>
       </c>
-      <c r="R5" s="158"/>
+      <c r="R5" s="160"/>
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25072,34 +25072,34 @@
       <c r="D49" s="131" t="s">
         <v>541</v>
       </c>
-      <c r="E49" s="161">
+      <c r="E49" s="155">
         <v>30.75</v>
       </c>
-      <c r="F49" s="159"/>
+      <c r="F49" s="161"/>
       <c r="G49" s="162">
         <v>44.59</v>
       </c>
-      <c r="H49" s="159"/>
-      <c r="I49" s="159">
+      <c r="H49" s="161"/>
+      <c r="I49" s="161">
         <v>45.04</v>
       </c>
-      <c r="J49" s="159"/>
-      <c r="K49" s="159">
+      <c r="J49" s="161"/>
+      <c r="K49" s="161">
         <v>48.32</v>
       </c>
-      <c r="L49" s="159"/>
-      <c r="M49" s="159">
+      <c r="L49" s="161"/>
+      <c r="M49" s="161">
         <v>47.61</v>
       </c>
-      <c r="N49" s="159"/>
-      <c r="O49" s="159">
+      <c r="N49" s="161"/>
+      <c r="O49" s="161">
         <v>45.52</v>
       </c>
-      <c r="P49" s="159"/>
-      <c r="Q49" s="159">
+      <c r="P49" s="161"/>
+      <c r="Q49" s="161">
         <v>49.19</v>
       </c>
-      <c r="R49" s="159"/>
+      <c r="R49" s="161"/>
     </row>
     <row r="50" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
@@ -25108,34 +25108,34 @@
       <c r="D50" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="E50" s="161">
+      <c r="E50" s="155">
         <v>48483</v>
       </c>
-      <c r="F50" s="159"/>
-      <c r="G50" s="161">
+      <c r="F50" s="161"/>
+      <c r="G50" s="155">
         <v>18474</v>
       </c>
-      <c r="H50" s="159"/>
-      <c r="I50" s="161">
+      <c r="H50" s="161"/>
+      <c r="I50" s="155">
         <v>18474</v>
       </c>
-      <c r="J50" s="159"/>
-      <c r="K50" s="161">
+      <c r="J50" s="161"/>
+      <c r="K50" s="155">
         <v>18474</v>
       </c>
-      <c r="L50" s="159"/>
-      <c r="M50" s="159">
+      <c r="L50" s="161"/>
+      <c r="M50" s="161">
         <v>17441</v>
       </c>
-      <c r="N50" s="159"/>
-      <c r="O50" s="159">
+      <c r="N50" s="161"/>
+      <c r="O50" s="161">
         <v>12670</v>
       </c>
-      <c r="P50" s="159"/>
-      <c r="Q50" s="159">
+      <c r="P50" s="161"/>
+      <c r="Q50" s="161">
         <v>16764</v>
       </c>
-      <c r="R50" s="159"/>
+      <c r="R50" s="161"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
@@ -25183,6 +25183,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="Q49:R49"/>
     <mergeCell ref="E50:F50"/>
     <mergeCell ref="G50:H50"/>
@@ -25197,14 +25205,6 @@
     <mergeCell ref="K49:L49"/>
     <mergeCell ref="M49:N49"/>
     <mergeCell ref="O49:P49"/>
-    <mergeCell ref="E4:R4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="portrait" r:id="rId1"/>
@@ -28942,18 +28942,18 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="155" t="s">
+      <c r="E4" s="157" t="s">
         <v>483</v>
       </c>
-      <c r="F4" s="156"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="156"/>
-      <c r="I4" s="156"/>
-      <c r="J4" s="156"/>
-      <c r="K4" s="156"/>
-      <c r="L4" s="156"/>
-      <c r="M4" s="156"/>
-      <c r="N4" s="156"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="158"/>
+      <c r="J4" s="158"/>
+      <c r="K4" s="158"/>
+      <c r="L4" s="158"/>
+      <c r="M4" s="158"/>
+      <c r="N4" s="158"/>
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -28963,26 +28963,26 @@
       <c r="D5" s="126" t="s">
         <v>382</v>
       </c>
-      <c r="E5" s="157" t="s">
+      <c r="E5" s="159" t="s">
         <v>513</v>
       </c>
-      <c r="F5" s="158"/>
-      <c r="G5" s="157" t="s">
+      <c r="F5" s="160"/>
+      <c r="G5" s="159" t="s">
         <v>514</v>
       </c>
-      <c r="H5" s="158"/>
-      <c r="I5" s="157" t="s">
+      <c r="H5" s="160"/>
+      <c r="I5" s="159" t="s">
         <v>515</v>
       </c>
-      <c r="J5" s="158"/>
-      <c r="K5" s="157" t="s">
+      <c r="J5" s="160"/>
+      <c r="K5" s="159" t="s">
         <v>516</v>
       </c>
-      <c r="L5" s="158"/>
-      <c r="M5" s="157" t="s">
+      <c r="L5" s="160"/>
+      <c r="M5" s="159" t="s">
         <v>517</v>
       </c>
-      <c r="N5" s="158"/>
+      <c r="N5" s="160"/>
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -30416,26 +30416,26 @@
       <c r="D44" s="131" t="s">
         <v>541</v>
       </c>
-      <c r="E44" s="161">
+      <c r="E44" s="155">
         <v>27.21</v>
       </c>
-      <c r="F44" s="160"/>
-      <c r="G44" s="161">
+      <c r="F44" s="156"/>
+      <c r="G44" s="155">
         <v>37.24</v>
       </c>
-      <c r="H44" s="160"/>
-      <c r="I44" s="161">
+      <c r="H44" s="156"/>
+      <c r="I44" s="155">
         <v>40.03</v>
       </c>
-      <c r="J44" s="160"/>
-      <c r="K44" s="161">
+      <c r="J44" s="156"/>
+      <c r="K44" s="155">
         <v>43.15</v>
       </c>
-      <c r="L44" s="160"/>
-      <c r="M44" s="161">
+      <c r="L44" s="156"/>
+      <c r="M44" s="155">
         <v>43.93</v>
       </c>
-      <c r="N44" s="160"/>
+      <c r="N44" s="156"/>
     </row>
     <row r="45" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
@@ -30444,26 +30444,26 @@
       <c r="D45" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="E45" s="161">
+      <c r="E45" s="155">
         <v>48483</v>
       </c>
-      <c r="F45" s="160"/>
-      <c r="G45" s="161">
+      <c r="F45" s="156"/>
+      <c r="G45" s="155">
         <v>46267</v>
       </c>
-      <c r="H45" s="160"/>
-      <c r="I45" s="161">
+      <c r="H45" s="156"/>
+      <c r="I45" s="155">
         <v>44046</v>
       </c>
-      <c r="J45" s="160"/>
-      <c r="K45" s="161">
+      <c r="J45" s="156"/>
+      <c r="K45" s="155">
         <v>30051</v>
       </c>
-      <c r="L45" s="160"/>
-      <c r="M45" s="161">
+      <c r="L45" s="156"/>
+      <c r="M45" s="155">
         <v>25612</v>
       </c>
-      <c r="N45" s="160"/>
+      <c r="N45" s="156"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
@@ -30501,22 +30501,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
     <mergeCell ref="E4:N4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="M45:N45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="portrait" r:id="rId1"/>
@@ -30572,22 +30572,22 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="155" t="s">
+      <c r="E4" s="157" t="s">
         <v>483</v>
       </c>
-      <c r="F4" s="156"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="156"/>
-      <c r="I4" s="156"/>
-      <c r="J4" s="156"/>
-      <c r="K4" s="156"/>
-      <c r="L4" s="156"/>
-      <c r="M4" s="156"/>
-      <c r="N4" s="156"/>
-      <c r="O4" s="156"/>
-      <c r="P4" s="156"/>
-      <c r="Q4" s="156"/>
-      <c r="R4" s="156"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="158"/>
+      <c r="J4" s="158"/>
+      <c r="K4" s="158"/>
+      <c r="L4" s="158"/>
+      <c r="M4" s="158"/>
+      <c r="N4" s="158"/>
+      <c r="O4" s="158"/>
+      <c r="P4" s="158"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="158"/>
       <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -30597,34 +30597,34 @@
       <c r="D5" s="126" t="s">
         <v>382</v>
       </c>
-      <c r="E5" s="157" t="s">
+      <c r="E5" s="159" t="s">
         <v>513</v>
       </c>
-      <c r="F5" s="158"/>
-      <c r="G5" s="157" t="s">
+      <c r="F5" s="160"/>
+      <c r="G5" s="159" t="s">
         <v>514</v>
       </c>
-      <c r="H5" s="158"/>
-      <c r="I5" s="157" t="s">
+      <c r="H5" s="160"/>
+      <c r="I5" s="159" t="s">
         <v>515</v>
       </c>
-      <c r="J5" s="158"/>
-      <c r="K5" s="157" t="s">
+      <c r="J5" s="160"/>
+      <c r="K5" s="159" t="s">
         <v>516</v>
       </c>
-      <c r="L5" s="158"/>
-      <c r="M5" s="157" t="s">
+      <c r="L5" s="160"/>
+      <c r="M5" s="159" t="s">
         <v>517</v>
       </c>
-      <c r="N5" s="158"/>
-      <c r="O5" s="157" t="s">
+      <c r="N5" s="160"/>
+      <c r="O5" s="159" t="s">
         <v>518</v>
       </c>
-      <c r="P5" s="158"/>
-      <c r="Q5" s="157" t="s">
+      <c r="P5" s="160"/>
+      <c r="Q5" s="159" t="s">
         <v>519</v>
       </c>
-      <c r="R5" s="158"/>
+      <c r="R5" s="160"/>
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -33506,34 +33506,34 @@
       <c r="D64" s="131" t="s">
         <v>541</v>
       </c>
-      <c r="E64" s="161">
+      <c r="E64" s="155">
         <v>27.21</v>
       </c>
-      <c r="F64" s="160"/>
+      <c r="F64" s="156"/>
       <c r="G64" s="162">
         <v>41.14</v>
       </c>
-      <c r="H64" s="160"/>
-      <c r="I64" s="159">
+      <c r="H64" s="156"/>
+      <c r="I64" s="161">
         <v>42.61</v>
       </c>
-      <c r="J64" s="160"/>
-      <c r="K64" s="159">
+      <c r="J64" s="156"/>
+      <c r="K64" s="161">
         <v>45.37</v>
       </c>
-      <c r="L64" s="160"/>
-      <c r="M64" s="159">
+      <c r="L64" s="156"/>
+      <c r="M64" s="161">
         <v>49.6</v>
       </c>
-      <c r="N64" s="160"/>
-      <c r="O64" s="159">
+      <c r="N64" s="156"/>
+      <c r="O64" s="161">
         <v>46.93</v>
       </c>
-      <c r="P64" s="160"/>
-      <c r="Q64" s="159">
+      <c r="P64" s="156"/>
+      <c r="Q64" s="161">
         <v>48.15</v>
       </c>
-      <c r="R64" s="160"/>
+      <c r="R64" s="156"/>
     </row>
     <row r="65" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
@@ -33542,34 +33542,34 @@
       <c r="D65" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="E65" s="161">
+      <c r="E65" s="155">
         <v>48483</v>
       </c>
-      <c r="F65" s="160"/>
-      <c r="G65" s="161">
+      <c r="F65" s="156"/>
+      <c r="G65" s="155">
         <v>17492</v>
       </c>
-      <c r="H65" s="160"/>
-      <c r="I65" s="161">
+      <c r="H65" s="156"/>
+      <c r="I65" s="155">
         <v>17492</v>
       </c>
-      <c r="J65" s="160"/>
-      <c r="K65" s="161">
+      <c r="J65" s="156"/>
+      <c r="K65" s="155">
         <v>17492</v>
       </c>
-      <c r="L65" s="160"/>
-      <c r="M65" s="159">
+      <c r="L65" s="156"/>
+      <c r="M65" s="161">
         <v>15660</v>
       </c>
-      <c r="N65" s="160"/>
-      <c r="O65" s="159">
+      <c r="N65" s="156"/>
+      <c r="O65" s="161">
         <v>11944</v>
       </c>
-      <c r="P65" s="160"/>
-      <c r="Q65" s="159">
+      <c r="P65" s="156"/>
+      <c r="Q65" s="161">
         <v>15422</v>
       </c>
-      <c r="R65" s="160"/>
+      <c r="R65" s="156"/>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
@@ -33617,14 +33617,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E4:R4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="Q64:R64"/>
     <mergeCell ref="E65:F65"/>
     <mergeCell ref="G65:H65"/>
@@ -33639,6 +33631,14 @@
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="M64:N64"/>
     <mergeCell ref="O64:P64"/>
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="portrait" r:id="rId1"/>

</xml_diff>